<commit_message>
Updated Deletereason description - Database-structure
</commit_message>
<xml_diff>
--- a/Draft/Datenbankstruktur.xlsx
+++ b/Draft/Datenbankstruktur.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="260">
   <si>
     <t>Datenbankstruktur</t>
   </si>
@@ -1409,6 +1409,12 @@
   </si>
   <si>
     <t>Pfad zum Smiley</t>
+  </si>
+  <si>
+    <t>Timestamp per Zeichen vom Löschgrund getrennt</t>
+  </si>
+  <si>
+    <t>{TIMESTAMP},TEXT</t>
   </si>
 </sst>
 </file>
@@ -1798,82 +1804,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1887,12 +1821,6 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1901,24 +1829,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1939,16 +1849,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1957,6 +1858,111 @@
     <xf numFmtId="0" fontId="8" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2271,21 +2277,21 @@
   <sheetData>
     <row r="1" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="73" t="s">
+      <c r="B1" s="38" t="s">
         <v>201</v>
       </c>
-      <c r="C1" s="59"/>
+      <c r="C1" s="27"/>
       <c r="D1" s="2"/>
       <c r="E1" s="3"/>
     </row>
     <row r="2" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="49"/>
-      <c r="B2" s="4" t="s">
+      <c r="A2" s="23"/>
+      <c r="B2" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="68"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="36"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="3"/>
@@ -2296,75 +2302,75 @@
       <c r="M2" s="3"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="47"/>
-      <c r="B3" s="7" t="s">
+      <c r="A3" s="21"/>
+      <c r="B3" s="75" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="27" t="s">
+      <c r="C3" s="76"/>
+      <c r="D3" s="77" t="s">
         <v>200</v>
       </c>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="44"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="57"/>
+      <c r="G3" s="58"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="47"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="28" t="s">
+      <c r="A4" s="21"/>
+      <c r="B4" s="55"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="29"/>
+      <c r="E4" s="59"/>
+      <c r="F4" s="59"/>
+      <c r="G4" s="60"/>
     </row>
     <row r="5" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="47"/>
-      <c r="B5" s="15" t="s">
+      <c r="A5" s="21"/>
+      <c r="B5" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="20" t="s">
+      <c r="D5" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="10"/>
+      <c r="E5" s="4"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="47"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="11"/>
+      <c r="A6" s="21"/>
+      <c r="B6" s="44"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="62"/>
+      <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="47"/>
-      <c r="B7" s="31" t="s">
+      <c r="A7" s="21"/>
+      <c r="B7" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="32" t="s">
+      <c r="C7" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D7" s="33" t="s">
+      <c r="D7" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="E7" s="11"/>
+      <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="47"/>
-      <c r="B8" s="34" t="s">
+      <c r="A8" s="21"/>
+      <c r="B8" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="35" t="s">
+      <c r="C8" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="D8" s="36"/>
+      <c r="D8" s="12"/>
     </row>
     <row r="9" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="66"/>
-      <c r="B9" s="74"/>
+      <c r="A9" s="34"/>
+      <c r="B9" s="39"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -2372,292 +2378,292 @@
       <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="47"/>
-      <c r="B10" s="9" t="s">
+      <c r="A10" s="21"/>
+      <c r="B10" s="53" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="69"/>
-      <c r="D10" s="43" t="s">
+      <c r="C10" s="54"/>
+      <c r="D10" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="43"/>
-      <c r="F10" s="43"/>
-      <c r="G10" s="44"/>
+      <c r="E10" s="57"/>
+      <c r="F10" s="57"/>
+      <c r="G10" s="58"/>
     </row>
     <row r="11" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="47"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="28" t="s">
+      <c r="A11" s="21"/>
+      <c r="B11" s="55"/>
+      <c r="C11" s="56"/>
+      <c r="D11" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="29"/>
+      <c r="E11" s="59"/>
+      <c r="F11" s="59"/>
+      <c r="G11" s="60"/>
     </row>
     <row r="12" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="47"/>
-      <c r="B12" s="15" t="s">
+      <c r="A12" s="21"/>
+      <c r="B12" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="C12" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="19" t="s">
+      <c r="D12" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="18" t="s">
+      <c r="E12" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="F12" s="19" t="s">
+      <c r="F12" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="G12" s="18" t="s">
+      <c r="G12" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="H12" s="20" t="s">
+      <c r="H12" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="I12" s="10"/>
+      <c r="I12" s="4"/>
     </row>
     <row r="13" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="47"/>
-      <c r="B13" s="16"/>
-      <c r="C13" s="26"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="26"/>
-      <c r="F13" s="25"/>
-      <c r="G13" s="26"/>
-      <c r="H13" s="21"/>
-      <c r="I13" s="10"/>
+      <c r="A13" s="21"/>
+      <c r="B13" s="44"/>
+      <c r="C13" s="49"/>
+      <c r="D13" s="50"/>
+      <c r="E13" s="49"/>
+      <c r="F13" s="50"/>
+      <c r="G13" s="49"/>
+      <c r="H13" s="62"/>
+      <c r="I13" s="4"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="47"/>
-      <c r="B14" s="31" t="s">
+      <c r="A14" s="21"/>
+      <c r="B14" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="32" t="s">
+      <c r="C14" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="31" t="s">
+      <c r="D14" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="E14" s="32" t="s">
+      <c r="E14" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="F14" s="31" t="s">
+      <c r="F14" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="G14" s="40" t="s">
+      <c r="G14" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="H14" s="33" t="s">
+      <c r="H14" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="I14" s="30"/>
+      <c r="I14" s="6"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="48"/>
-      <c r="B15" s="34"/>
-      <c r="C15" s="35"/>
-      <c r="D15" s="38" t="s">
+      <c r="A15" s="22"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="E15" s="35" t="s">
+      <c r="E15" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="F15" s="38" t="s">
+      <c r="F15" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="G15" s="35"/>
-      <c r="H15" s="36"/>
-      <c r="I15" s="30"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="6"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="66"/>
-      <c r="B16" s="74"/>
-      <c r="C16" s="70"/>
-      <c r="D16" s="70"/>
-      <c r="E16" s="70"/>
-      <c r="F16" s="70"/>
-      <c r="G16" s="70"/>
+      <c r="A16" s="34"/>
+      <c r="B16" s="39"/>
+      <c r="C16" s="37"/>
+      <c r="D16" s="37"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="37"/>
+      <c r="G16" s="37"/>
     </row>
     <row r="17" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="47"/>
-      <c r="B17" s="9" t="s">
+      <c r="A17" s="21"/>
+      <c r="B17" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="69"/>
-      <c r="D17" s="43" t="s">
+      <c r="C17" s="54"/>
+      <c r="D17" s="57" t="s">
         <v>199</v>
       </c>
-      <c r="E17" s="43"/>
-      <c r="F17" s="43"/>
-      <c r="G17" s="44"/>
+      <c r="E17" s="57"/>
+      <c r="F17" s="57"/>
+      <c r="G17" s="58"/>
     </row>
     <row r="18" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="47"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="28" t="s">
+      <c r="A18" s="21"/>
+      <c r="B18" s="55"/>
+      <c r="C18" s="56"/>
+      <c r="D18" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="E18" s="28"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="29"/>
+      <c r="E18" s="59"/>
+      <c r="F18" s="59"/>
+      <c r="G18" s="60"/>
     </row>
     <row r="19" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="47"/>
-      <c r="B19" s="15" t="s">
+      <c r="A19" s="21"/>
+      <c r="B19" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="18" t="s">
+      <c r="C19" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="D19" s="19" t="s">
+      <c r="D19" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="E19" s="18" t="s">
+      <c r="E19" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="F19" s="19" t="s">
+      <c r="F19" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="G19" s="22" t="s">
+      <c r="G19" s="51" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="47"/>
-      <c r="B20" s="16"/>
-      <c r="C20" s="26"/>
-      <c r="D20" s="25"/>
-      <c r="E20" s="26"/>
-      <c r="F20" s="25"/>
-      <c r="G20" s="23"/>
+      <c r="A20" s="21"/>
+      <c r="B20" s="44"/>
+      <c r="C20" s="49"/>
+      <c r="D20" s="50"/>
+      <c r="E20" s="49"/>
+      <c r="F20" s="50"/>
+      <c r="G20" s="52"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="47"/>
-      <c r="B21" s="31" t="s">
+      <c r="A21" s="21"/>
+      <c r="B21" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C21" s="32" t="s">
+      <c r="C21" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D21" s="31" t="s">
+      <c r="D21" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="E21" s="32" t="s">
+      <c r="E21" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="F21" s="31" t="s">
+      <c r="F21" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="G21" s="37" t="s">
+      <c r="G21" s="13" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="48"/>
-      <c r="B22" s="34"/>
-      <c r="C22" s="35"/>
-      <c r="D22" s="38"/>
-      <c r="E22" s="35"/>
-      <c r="F22" s="38"/>
-      <c r="G22" s="39" t="s">
+      <c r="A22" s="22"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="15" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="66"/>
-      <c r="B23" s="74"/>
-      <c r="C23" s="70"/>
-      <c r="D23" s="70"/>
-      <c r="E23" s="70"/>
-      <c r="F23" s="70"/>
-      <c r="G23" s="70"/>
+      <c r="A23" s="34"/>
+      <c r="B23" s="39"/>
+      <c r="C23" s="37"/>
+      <c r="D23" s="37"/>
+      <c r="E23" s="37"/>
+      <c r="F23" s="37"/>
+      <c r="G23" s="37"/>
     </row>
     <row r="24" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="48"/>
-      <c r="B24" s="9" t="s">
+      <c r="A24" s="22"/>
+      <c r="B24" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="C24" s="69"/>
-      <c r="D24" s="43" t="s">
+      <c r="C24" s="54"/>
+      <c r="D24" s="57" t="s">
         <v>197</v>
       </c>
-      <c r="E24" s="43"/>
-      <c r="F24" s="43"/>
-      <c r="G24" s="44"/>
+      <c r="E24" s="57"/>
+      <c r="F24" s="57"/>
+      <c r="G24" s="58"/>
     </row>
     <row r="25" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="48"/>
-      <c r="B25" s="12"/>
-      <c r="C25" s="13"/>
-      <c r="D25" s="28" t="s">
+      <c r="A25" s="22"/>
+      <c r="B25" s="55"/>
+      <c r="C25" s="56"/>
+      <c r="D25" s="59" t="s">
         <v>57</v>
       </c>
-      <c r="E25" s="28"/>
-      <c r="F25" s="28"/>
-      <c r="G25" s="29"/>
+      <c r="E25" s="59"/>
+      <c r="F25" s="59"/>
+      <c r="G25" s="60"/>
     </row>
     <row r="26" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="48"/>
-      <c r="B26" s="15" t="s">
+      <c r="A26" s="22"/>
+      <c r="B26" s="43" t="s">
         <v>46</v>
       </c>
-      <c r="C26" s="18" t="s">
+      <c r="C26" s="45" t="s">
         <v>47</v>
       </c>
-      <c r="D26" s="20" t="s">
+      <c r="D26" s="61" t="s">
         <v>48</v>
       </c>
-      <c r="E26" s="10"/>
-      <c r="F26" s="10"/>
-      <c r="G26" s="10"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
     </row>
     <row r="27" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="48"/>
-      <c r="B27" s="16"/>
-      <c r="C27" s="26"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="10"/>
-      <c r="G27" s="10"/>
+      <c r="A27" s="22"/>
+      <c r="B27" s="44"/>
+      <c r="C27" s="49"/>
+      <c r="D27" s="62"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="47"/>
-      <c r="B28" s="31" t="s">
+      <c r="A28" s="21"/>
+      <c r="B28" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C28" s="32" t="s">
+      <c r="C28" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="D28" s="33" t="s">
+      <c r="D28" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="E28" s="45"/>
-      <c r="F28" s="46"/>
-      <c r="G28" s="45"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="19"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" s="50"/>
-      <c r="B29" s="34" t="s">
+      <c r="A29" s="24"/>
+      <c r="B29" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="C29" s="35" t="s">
+      <c r="C29" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="D29" s="36" t="s">
+      <c r="D29" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="E29" s="45"/>
-      <c r="F29" s="46"/>
-      <c r="G29" s="45"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="19"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" s="66"/>
-      <c r="B30" s="74"/>
+      <c r="A30" s="34"/>
+      <c r="B30" s="39"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
@@ -2665,29 +2671,29 @@
       <c r="G30" s="2"/>
     </row>
     <row r="31" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="48"/>
-      <c r="B31" s="9" t="s">
+      <c r="A31" s="22"/>
+      <c r="B31" s="53" t="s">
         <v>56</v>
       </c>
-      <c r="C31" s="69"/>
-      <c r="D31" s="43" t="s">
+      <c r="C31" s="54"/>
+      <c r="D31" s="57" t="s">
         <v>198</v>
       </c>
-      <c r="E31" s="43"/>
-      <c r="F31" s="43"/>
-      <c r="G31" s="44"/>
+      <c r="E31" s="57"/>
+      <c r="F31" s="57"/>
+      <c r="G31" s="58"/>
     </row>
     <row r="32" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="48"/>
-      <c r="B32" s="12"/>
-      <c r="C32" s="13"/>
-      <c r="D32" s="28" t="s">
+      <c r="A32" s="22"/>
+      <c r="B32" s="55"/>
+      <c r="C32" s="56"/>
+      <c r="D32" s="59" t="s">
         <v>58</v>
       </c>
-      <c r="E32" s="28"/>
-      <c r="F32" s="28"/>
-      <c r="G32" s="29"/>
-      <c r="H32" s="52"/>
+      <c r="E32" s="59"/>
+      <c r="F32" s="59"/>
+      <c r="G32" s="60"/>
+      <c r="H32" s="26"/>
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>
@@ -2695,201 +2701,201 @@
       <c r="M32" s="2"/>
     </row>
     <row r="33" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="48"/>
-      <c r="B33" s="15" t="s">
+      <c r="A33" s="22"/>
+      <c r="B33" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="C33" s="18" t="s">
+      <c r="C33" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="D33" s="19" t="s">
+      <c r="D33" s="47" t="s">
         <v>60</v>
       </c>
-      <c r="E33" s="18" t="s">
+      <c r="E33" s="45" t="s">
         <v>61</v>
       </c>
-      <c r="F33" s="19" t="s">
+      <c r="F33" s="47" t="s">
         <v>46</v>
       </c>
-      <c r="G33" s="18" t="s">
+      <c r="G33" s="45" t="s">
         <v>62</v>
       </c>
-      <c r="H33" s="19" t="s">
+      <c r="H33" s="47" t="s">
         <v>63</v>
       </c>
-      <c r="I33" s="18" t="s">
+      <c r="I33" s="45" t="s">
         <v>65</v>
       </c>
-      <c r="J33" s="19" t="s">
+      <c r="J33" s="47" t="s">
         <v>66</v>
       </c>
-      <c r="K33" s="18" t="s">
+      <c r="K33" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="L33" s="19" t="s">
+      <c r="L33" s="47" t="s">
         <v>67</v>
       </c>
-      <c r="M33" s="22" t="s">
+      <c r="M33" s="51" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="34" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="48"/>
-      <c r="B34" s="16"/>
-      <c r="C34" s="26"/>
-      <c r="D34" s="25"/>
-      <c r="E34" s="26"/>
-      <c r="F34" s="25"/>
-      <c r="G34" s="26"/>
-      <c r="H34" s="25"/>
-      <c r="I34" s="26"/>
-      <c r="J34" s="25"/>
-      <c r="K34" s="26"/>
-      <c r="L34" s="25"/>
-      <c r="M34" s="23"/>
+      <c r="A34" s="22"/>
+      <c r="B34" s="44"/>
+      <c r="C34" s="49"/>
+      <c r="D34" s="50"/>
+      <c r="E34" s="49"/>
+      <c r="F34" s="50"/>
+      <c r="G34" s="49"/>
+      <c r="H34" s="50"/>
+      <c r="I34" s="49"/>
+      <c r="J34" s="50"/>
+      <c r="K34" s="49"/>
+      <c r="L34" s="50"/>
+      <c r="M34" s="52"/>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A35" s="47"/>
-      <c r="B35" s="31" t="s">
+      <c r="A35" s="21"/>
+      <c r="B35" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C35" s="32"/>
-      <c r="D35" s="51" t="s">
+      <c r="C35" s="8"/>
+      <c r="D35" s="25" t="s">
         <v>81</v>
       </c>
-      <c r="E35" s="32"/>
-      <c r="F35" s="51"/>
-      <c r="G35" s="32"/>
-      <c r="H35" s="51" t="s">
+      <c r="E35" s="8"/>
+      <c r="F35" s="25"/>
+      <c r="G35" s="8"/>
+      <c r="H35" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="I35" s="32" t="s">
+      <c r="I35" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="J35" s="51" t="s">
+      <c r="J35" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="K35" s="32" t="s">
+      <c r="K35" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="L35" s="51"/>
-      <c r="M35" s="37"/>
+      <c r="L35" s="25"/>
+      <c r="M35" s="13"/>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A36" s="50"/>
-      <c r="B36" s="34"/>
-      <c r="C36" s="35"/>
-      <c r="D36" s="38" t="s">
+      <c r="A36" s="24"/>
+      <c r="B36" s="10"/>
+      <c r="C36" s="11"/>
+      <c r="D36" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="E36" s="35"/>
-      <c r="F36" s="38" t="s">
+      <c r="E36" s="11"/>
+      <c r="F36" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="G36" s="35"/>
-      <c r="H36" s="38"/>
-      <c r="I36" s="35" t="s">
+      <c r="G36" s="11"/>
+      <c r="H36" s="14"/>
+      <c r="I36" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="J36" s="38" t="s">
+      <c r="J36" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="K36" s="35" t="s">
+      <c r="K36" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="L36" s="38"/>
-      <c r="M36" s="39"/>
+      <c r="L36" s="14"/>
+      <c r="M36" s="15"/>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A37" s="66"/>
-      <c r="B37" s="74"/>
-      <c r="C37" s="70"/>
-      <c r="D37" s="70"/>
-      <c r="E37" s="70"/>
-      <c r="F37" s="70"/>
-      <c r="G37" s="70"/>
+      <c r="A37" s="34"/>
+      <c r="B37" s="39"/>
+      <c r="C37" s="37"/>
+      <c r="D37" s="37"/>
+      <c r="E37" s="37"/>
+      <c r="F37" s="37"/>
+      <c r="G37" s="37"/>
     </row>
     <row r="38" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="48"/>
-      <c r="B38" s="9" t="s">
+      <c r="A38" s="22"/>
+      <c r="B38" s="53" t="s">
         <v>75</v>
       </c>
-      <c r="C38" s="69"/>
-      <c r="D38" s="43" t="s">
+      <c r="C38" s="54"/>
+      <c r="D38" s="57" t="s">
         <v>196</v>
       </c>
-      <c r="E38" s="43"/>
-      <c r="F38" s="43"/>
-      <c r="G38" s="44"/>
+      <c r="E38" s="57"/>
+      <c r="F38" s="57"/>
+      <c r="G38" s="58"/>
     </row>
     <row r="39" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="48"/>
-      <c r="B39" s="12"/>
-      <c r="C39" s="13"/>
-      <c r="D39" s="28" t="s">
+      <c r="A39" s="22"/>
+      <c r="B39" s="55"/>
+      <c r="C39" s="56"/>
+      <c r="D39" s="59" t="s">
         <v>79</v>
       </c>
-      <c r="E39" s="28"/>
-      <c r="F39" s="28"/>
-      <c r="G39" s="29"/>
+      <c r="E39" s="59"/>
+      <c r="F39" s="59"/>
+      <c r="G39" s="60"/>
     </row>
     <row r="40" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="48"/>
-      <c r="B40" s="15" t="s">
+      <c r="A40" s="22"/>
+      <c r="B40" s="43" t="s">
         <v>77</v>
       </c>
-      <c r="C40" s="18" t="s">
+      <c r="C40" s="45" t="s">
         <v>47</v>
       </c>
-      <c r="D40" s="20" t="s">
+      <c r="D40" s="61" t="s">
         <v>48</v>
       </c>
-      <c r="E40" s="10"/>
-      <c r="F40" s="10"/>
-      <c r="G40" s="10"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="4"/>
     </row>
     <row r="41" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="48"/>
-      <c r="B41" s="16"/>
-      <c r="C41" s="26"/>
-      <c r="D41" s="21"/>
-      <c r="E41" s="10"/>
-      <c r="F41" s="10"/>
-      <c r="G41" s="10"/>
+      <c r="A41" s="22"/>
+      <c r="B41" s="44"/>
+      <c r="C41" s="49"/>
+      <c r="D41" s="62"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
+      <c r="G41" s="4"/>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A42" s="47"/>
-      <c r="B42" s="31" t="s">
+      <c r="A42" s="21"/>
+      <c r="B42" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="C42" s="32" t="s">
+      <c r="C42" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="D42" s="33" t="s">
+      <c r="D42" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="E42" s="45"/>
-      <c r="F42" s="46"/>
-      <c r="G42" s="45"/>
+      <c r="E42" s="19"/>
+      <c r="F42" s="20"/>
+      <c r="G42" s="19"/>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A43" s="50"/>
-      <c r="B43" s="34" t="s">
+      <c r="A43" s="24"/>
+      <c r="B43" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="C43" s="35" t="s">
+      <c r="C43" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="D43" s="36" t="s">
+      <c r="D43" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="E43" s="45"/>
-      <c r="F43" s="46"/>
-      <c r="G43" s="45"/>
+      <c r="E43" s="19"/>
+      <c r="F43" s="20"/>
+      <c r="G43" s="19"/>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A44" s="66"/>
-      <c r="B44" s="74"/>
+      <c r="A44" s="34"/>
+      <c r="B44" s="39"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
@@ -2897,564 +2903,564 @@
       <c r="G44" s="2"/>
     </row>
     <row r="45" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="47"/>
-      <c r="B45" s="9" t="s">
+      <c r="A45" s="21"/>
+      <c r="B45" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="C45" s="69"/>
-      <c r="D45" s="43" t="s">
+      <c r="C45" s="54"/>
+      <c r="D45" s="57" t="s">
         <v>195</v>
       </c>
-      <c r="E45" s="43"/>
-      <c r="F45" s="43"/>
-      <c r="G45" s="44"/>
+      <c r="E45" s="57"/>
+      <c r="F45" s="57"/>
+      <c r="G45" s="58"/>
     </row>
     <row r="46" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="47"/>
-      <c r="B46" s="12"/>
-      <c r="C46" s="13"/>
-      <c r="D46" s="28" t="s">
+      <c r="A46" s="21"/>
+      <c r="B46" s="55"/>
+      <c r="C46" s="56"/>
+      <c r="D46" s="59" t="s">
         <v>103</v>
       </c>
-      <c r="E46" s="28"/>
-      <c r="F46" s="28"/>
-      <c r="G46" s="29"/>
+      <c r="E46" s="59"/>
+      <c r="F46" s="59"/>
+      <c r="G46" s="60"/>
     </row>
     <row r="47" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="47"/>
-      <c r="B47" s="15" t="s">
+      <c r="A47" s="21"/>
+      <c r="B47" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="C47" s="18" t="s">
+      <c r="C47" s="45" t="s">
         <v>112</v>
       </c>
-      <c r="D47" s="19" t="s">
+      <c r="D47" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="E47" s="18" t="s">
+      <c r="E47" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="F47" s="19" t="s">
+      <c r="F47" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="G47" s="18" t="s">
+      <c r="G47" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="H47" s="19" t="s">
+      <c r="H47" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="I47" s="18" t="s">
+      <c r="I47" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="J47" s="19" t="s">
+      <c r="J47" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="K47" s="18" t="s">
+      <c r="K47" s="45" t="s">
         <v>119</v>
       </c>
-      <c r="L47" s="19" t="s">
+      <c r="L47" s="47" t="s">
         <v>120</v>
       </c>
-      <c r="M47" s="18" t="s">
+      <c r="M47" s="45" t="s">
         <v>121</v>
       </c>
-      <c r="N47" s="19" t="s">
+      <c r="N47" s="47" t="s">
         <v>134</v>
       </c>
-      <c r="O47" s="18" t="s">
+      <c r="O47" s="45" t="s">
         <v>122</v>
       </c>
-      <c r="P47" s="19" t="s">
+      <c r="P47" s="47" t="s">
         <v>123</v>
       </c>
-      <c r="Q47" s="22" t="s">
+      <c r="Q47" s="51" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="48" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="47"/>
-      <c r="B48" s="16"/>
-      <c r="C48" s="17"/>
-      <c r="D48" s="14"/>
-      <c r="E48" s="17"/>
-      <c r="F48" s="14"/>
-      <c r="G48" s="17"/>
-      <c r="H48" s="14"/>
-      <c r="I48" s="26"/>
-      <c r="J48" s="25"/>
-      <c r="K48" s="17"/>
-      <c r="L48" s="14"/>
-      <c r="M48" s="17"/>
-      <c r="N48" s="14"/>
-      <c r="O48" s="17"/>
-      <c r="P48" s="25"/>
-      <c r="Q48" s="23"/>
+      <c r="A48" s="21"/>
+      <c r="B48" s="44"/>
+      <c r="C48" s="46"/>
+      <c r="D48" s="48"/>
+      <c r="E48" s="46"/>
+      <c r="F48" s="48"/>
+      <c r="G48" s="46"/>
+      <c r="H48" s="48"/>
+      <c r="I48" s="49"/>
+      <c r="J48" s="50"/>
+      <c r="K48" s="46"/>
+      <c r="L48" s="48"/>
+      <c r="M48" s="46"/>
+      <c r="N48" s="48"/>
+      <c r="O48" s="46"/>
+      <c r="P48" s="50"/>
+      <c r="Q48" s="52"/>
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A49" s="47"/>
-      <c r="B49" s="31" t="s">
+      <c r="A49" s="21"/>
+      <c r="B49" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C49" s="32"/>
-      <c r="D49" s="31" t="s">
+      <c r="C49" s="8"/>
+      <c r="D49" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E49" s="32"/>
-      <c r="F49" s="31"/>
-      <c r="G49" s="32"/>
-      <c r="H49" s="31"/>
-      <c r="I49" s="40" t="s">
+      <c r="E49" s="8"/>
+      <c r="F49" s="7"/>
+      <c r="G49" s="8"/>
+      <c r="H49" s="7"/>
+      <c r="I49" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="J49" s="31" t="s">
+      <c r="J49" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="K49" s="32" t="s">
+      <c r="K49" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="L49" s="31"/>
-      <c r="M49" s="32"/>
-      <c r="N49" s="31"/>
-      <c r="O49" s="32"/>
-      <c r="P49" s="51"/>
-      <c r="Q49" s="37"/>
+      <c r="L49" s="7"/>
+      <c r="M49" s="8"/>
+      <c r="N49" s="7"/>
+      <c r="O49" s="8"/>
+      <c r="P49" s="25"/>
+      <c r="Q49" s="13"/>
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A50" s="47"/>
-      <c r="B50" s="34"/>
-      <c r="C50" s="35" t="s">
+      <c r="A50" s="21"/>
+      <c r="B50" s="10"/>
+      <c r="C50" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="D50" s="38"/>
-      <c r="E50" s="35"/>
-      <c r="F50" s="38"/>
-      <c r="G50" s="35"/>
-      <c r="H50" s="38"/>
-      <c r="I50" s="35"/>
-      <c r="J50" s="38"/>
-      <c r="K50" s="35"/>
-      <c r="L50" s="38"/>
-      <c r="M50" s="35"/>
-      <c r="N50" s="38"/>
-      <c r="O50" s="35"/>
-      <c r="P50" s="38"/>
-      <c r="Q50" s="39"/>
+      <c r="D50" s="14"/>
+      <c r="E50" s="11"/>
+      <c r="F50" s="14"/>
+      <c r="G50" s="11"/>
+      <c r="H50" s="14"/>
+      <c r="I50" s="11"/>
+      <c r="J50" s="14"/>
+      <c r="K50" s="11"/>
+      <c r="L50" s="14"/>
+      <c r="M50" s="11"/>
+      <c r="N50" s="14"/>
+      <c r="O50" s="11"/>
+      <c r="P50" s="14"/>
+      <c r="Q50" s="15"/>
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A51" s="66"/>
-      <c r="B51" s="74"/>
-      <c r="C51" s="70"/>
-      <c r="D51" s="70"/>
-      <c r="E51" s="70"/>
-      <c r="F51" s="70"/>
-      <c r="G51" s="70"/>
+      <c r="A51" s="34"/>
+      <c r="B51" s="39"/>
+      <c r="C51" s="37"/>
+      <c r="D51" s="37"/>
+      <c r="E51" s="37"/>
+      <c r="F51" s="37"/>
+      <c r="G51" s="37"/>
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A52" s="47"/>
-      <c r="B52" s="71" t="s">
+      <c r="A52" s="21"/>
+      <c r="B52" s="68" t="s">
         <v>83</v>
       </c>
-      <c r="C52" s="72"/>
-      <c r="D52" s="43" t="s">
+      <c r="C52" s="69"/>
+      <c r="D52" s="57" t="s">
         <v>194</v>
       </c>
-      <c r="E52" s="43"/>
-      <c r="F52" s="43"/>
-      <c r="G52" s="44"/>
+      <c r="E52" s="57"/>
+      <c r="F52" s="57"/>
+      <c r="G52" s="58"/>
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A53" s="47"/>
-      <c r="B53" s="53"/>
-      <c r="C53" s="54"/>
-      <c r="D53" s="28" t="s">
+      <c r="A53" s="21"/>
+      <c r="B53" s="70"/>
+      <c r="C53" s="71"/>
+      <c r="D53" s="59" t="s">
         <v>106</v>
       </c>
-      <c r="E53" s="28"/>
-      <c r="F53" s="28"/>
-      <c r="G53" s="29"/>
+      <c r="E53" s="59"/>
+      <c r="F53" s="59"/>
+      <c r="G53" s="60"/>
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A54" s="47"/>
-      <c r="B54" s="15" t="s">
+      <c r="A54" s="21"/>
+      <c r="B54" s="43" t="s">
         <v>84</v>
       </c>
-      <c r="C54" s="18" t="s">
+      <c r="C54" s="45" t="s">
         <v>46</v>
       </c>
-      <c r="D54" s="19" t="s">
+      <c r="D54" s="47" t="s">
         <v>85</v>
       </c>
-      <c r="E54" s="18" t="s">
+      <c r="E54" s="45" t="s">
         <v>86</v>
       </c>
-      <c r="F54" s="19" t="s">
+      <c r="F54" s="47" t="s">
         <v>88</v>
       </c>
-      <c r="G54" s="18" t="s">
+      <c r="G54" s="45" t="s">
         <v>87</v>
       </c>
-      <c r="H54" s="55" t="s">
+      <c r="H54" s="64" t="s">
         <v>89</v>
       </c>
-      <c r="I54" s="18" t="s">
+      <c r="I54" s="45" t="s">
         <v>90</v>
       </c>
-      <c r="J54" s="19" t="s">
+      <c r="J54" s="47" t="s">
         <v>91</v>
       </c>
-      <c r="K54" s="57" t="s">
+      <c r="K54" s="66" t="s">
         <v>92</v>
       </c>
-      <c r="L54" s="55" t="s">
+      <c r="L54" s="64" t="s">
         <v>93</v>
       </c>
-      <c r="M54" s="18" t="s">
+      <c r="M54" s="45" t="s">
         <v>94</v>
       </c>
-      <c r="N54" s="19" t="s">
+      <c r="N54" s="47" t="s">
         <v>95</v>
       </c>
-      <c r="O54" s="18" t="s">
+      <c r="O54" s="45" t="s">
         <v>96</v>
       </c>
-      <c r="P54" s="19" t="s">
+      <c r="P54" s="47" t="s">
         <v>97</v>
       </c>
-      <c r="Q54" s="18" t="s">
+      <c r="Q54" s="45" t="s">
         <v>100</v>
       </c>
-      <c r="R54" s="19" t="s">
+      <c r="R54" s="47" t="s">
         <v>99</v>
       </c>
-      <c r="S54" s="22" t="s">
+      <c r="S54" s="51" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="55" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A55" s="47"/>
-      <c r="B55" s="16"/>
-      <c r="C55" s="17"/>
-      <c r="D55" s="14"/>
-      <c r="E55" s="17"/>
-      <c r="F55" s="14"/>
-      <c r="G55" s="17"/>
-      <c r="H55" s="56"/>
-      <c r="I55" s="17"/>
-      <c r="J55" s="14"/>
-      <c r="K55" s="58"/>
-      <c r="L55" s="56"/>
-      <c r="M55" s="17"/>
-      <c r="N55" s="14"/>
-      <c r="O55" s="17"/>
-      <c r="P55" s="14"/>
-      <c r="Q55" s="17"/>
-      <c r="R55" s="14"/>
-      <c r="S55" s="23"/>
+      <c r="A55" s="21"/>
+      <c r="B55" s="44"/>
+      <c r="C55" s="46"/>
+      <c r="D55" s="48"/>
+      <c r="E55" s="46"/>
+      <c r="F55" s="48"/>
+      <c r="G55" s="46"/>
+      <c r="H55" s="65"/>
+      <c r="I55" s="46"/>
+      <c r="J55" s="48"/>
+      <c r="K55" s="67"/>
+      <c r="L55" s="65"/>
+      <c r="M55" s="46"/>
+      <c r="N55" s="48"/>
+      <c r="O55" s="46"/>
+      <c r="P55" s="48"/>
+      <c r="Q55" s="46"/>
+      <c r="R55" s="48"/>
+      <c r="S55" s="52"/>
     </row>
     <row r="56" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A56" s="47"/>
-      <c r="B56" s="31" t="s">
+      <c r="A56" s="21"/>
+      <c r="B56" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="C56" s="32" t="s">
+      <c r="C56" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="D56" s="31"/>
-      <c r="E56" s="32"/>
-      <c r="F56" s="31"/>
-      <c r="G56" s="32"/>
-      <c r="H56" s="31"/>
-      <c r="I56" s="32"/>
-      <c r="J56" s="31"/>
-      <c r="K56" s="32"/>
-      <c r="L56" s="31"/>
-      <c r="M56" s="32"/>
-      <c r="N56" s="31"/>
-      <c r="O56" s="32"/>
-      <c r="P56" s="31"/>
-      <c r="Q56" s="32" t="s">
+      <c r="D56" s="7"/>
+      <c r="E56" s="8"/>
+      <c r="F56" s="7"/>
+      <c r="G56" s="8"/>
+      <c r="H56" s="7"/>
+      <c r="I56" s="8"/>
+      <c r="J56" s="7"/>
+      <c r="K56" s="8"/>
+      <c r="L56" s="7"/>
+      <c r="M56" s="8"/>
+      <c r="N56" s="7"/>
+      <c r="O56" s="8"/>
+      <c r="P56" s="7"/>
+      <c r="Q56" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="R56" s="31" t="s">
+      <c r="R56" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="S56" s="37" t="s">
+      <c r="S56" s="13" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="57" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A57" s="47"/>
-      <c r="B57" s="34" t="s">
+      <c r="A57" s="21"/>
+      <c r="B57" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="C57" s="35" t="s">
+      <c r="C57" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="D57" s="38"/>
-      <c r="E57" s="35"/>
-      <c r="F57" s="38"/>
-      <c r="G57" s="35"/>
-      <c r="H57" s="38"/>
-      <c r="I57" s="35"/>
-      <c r="J57" s="38"/>
-      <c r="K57" s="35"/>
-      <c r="L57" s="38"/>
-      <c r="M57" s="35"/>
-      <c r="N57" s="38"/>
-      <c r="O57" s="35"/>
-      <c r="P57" s="38"/>
-      <c r="Q57" s="35"/>
-      <c r="R57" s="38"/>
-      <c r="S57" s="39"/>
+      <c r="D57" s="14"/>
+      <c r="E57" s="11"/>
+      <c r="F57" s="14"/>
+      <c r="G57" s="11"/>
+      <c r="H57" s="14"/>
+      <c r="I57" s="11"/>
+      <c r="J57" s="14"/>
+      <c r="K57" s="11"/>
+      <c r="L57" s="14"/>
+      <c r="M57" s="11"/>
+      <c r="N57" s="14"/>
+      <c r="O57" s="11"/>
+      <c r="P57" s="14"/>
+      <c r="Q57" s="11"/>
+      <c r="R57" s="14"/>
+      <c r="S57" s="15"/>
     </row>
     <row r="58" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A58" s="66"/>
-      <c r="B58" s="74"/>
-      <c r="C58" s="70"/>
-      <c r="D58" s="70"/>
-      <c r="E58" s="70"/>
-      <c r="F58" s="70"/>
-      <c r="G58" s="70"/>
+      <c r="A58" s="34"/>
+      <c r="B58" s="39"/>
+      <c r="C58" s="37"/>
+      <c r="D58" s="37"/>
+      <c r="E58" s="37"/>
+      <c r="F58" s="37"/>
+      <c r="G58" s="37"/>
     </row>
     <row r="59" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A59" s="47"/>
-      <c r="B59" s="71" t="s">
+      <c r="A59" s="21"/>
+      <c r="B59" s="68" t="s">
         <v>109</v>
       </c>
-      <c r="C59" s="72"/>
-      <c r="D59" s="43" t="s">
+      <c r="C59" s="69"/>
+      <c r="D59" s="57" t="s">
         <v>193</v>
       </c>
-      <c r="E59" s="43"/>
-      <c r="F59" s="43"/>
-      <c r="G59" s="44"/>
+      <c r="E59" s="57"/>
+      <c r="F59" s="57"/>
+      <c r="G59" s="58"/>
     </row>
     <row r="60" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A60" s="47"/>
-      <c r="B60" s="53"/>
-      <c r="C60" s="54"/>
-      <c r="D60" s="28" t="s">
+      <c r="A60" s="21"/>
+      <c r="B60" s="70"/>
+      <c r="C60" s="71"/>
+      <c r="D60" s="59" t="s">
         <v>111</v>
       </c>
-      <c r="E60" s="28"/>
-      <c r="F60" s="28"/>
-      <c r="G60" s="29"/>
+      <c r="E60" s="59"/>
+      <c r="F60" s="59"/>
+      <c r="G60" s="60"/>
     </row>
     <row r="61" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A61" s="47"/>
-      <c r="B61" s="15" t="s">
+      <c r="A61" s="21"/>
+      <c r="B61" s="43" t="s">
         <v>84</v>
       </c>
-      <c r="C61" s="18" t="s">
+      <c r="C61" s="45" t="s">
         <v>77</v>
       </c>
-      <c r="D61" s="19" t="s">
+      <c r="D61" s="47" t="s">
         <v>85</v>
       </c>
-      <c r="E61" s="18" t="s">
+      <c r="E61" s="45" t="s">
         <v>86</v>
       </c>
-      <c r="F61" s="19" t="s">
+      <c r="F61" s="47" t="s">
         <v>88</v>
       </c>
-      <c r="G61" s="18" t="s">
+      <c r="G61" s="45" t="s">
         <v>87</v>
       </c>
-      <c r="H61" s="55" t="s">
+      <c r="H61" s="64" t="s">
         <v>89</v>
       </c>
-      <c r="I61" s="18" t="s">
+      <c r="I61" s="45" t="s">
         <v>90</v>
       </c>
-      <c r="J61" s="19" t="s">
+      <c r="J61" s="47" t="s">
         <v>91</v>
       </c>
-      <c r="K61" s="57" t="s">
+      <c r="K61" s="66" t="s">
         <v>92</v>
       </c>
-      <c r="L61" s="55" t="s">
+      <c r="L61" s="64" t="s">
         <v>93</v>
       </c>
-      <c r="M61" s="18" t="s">
+      <c r="M61" s="45" t="s">
         <v>94</v>
       </c>
-      <c r="N61" s="19" t="s">
+      <c r="N61" s="47" t="s">
         <v>95</v>
       </c>
-      <c r="O61" s="18" t="s">
+      <c r="O61" s="45" t="s">
         <v>96</v>
       </c>
-      <c r="P61" s="19" t="s">
+      <c r="P61" s="47" t="s">
         <v>97</v>
       </c>
-      <c r="Q61" s="18" t="s">
+      <c r="Q61" s="45" t="s">
         <v>100</v>
       </c>
-      <c r="R61" s="19" t="s">
+      <c r="R61" s="47" t="s">
         <v>99</v>
       </c>
-      <c r="S61" s="22" t="s">
+      <c r="S61" s="51" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A62" s="47"/>
-      <c r="B62" s="16"/>
-      <c r="C62" s="17"/>
-      <c r="D62" s="14"/>
-      <c r="E62" s="17"/>
-      <c r="F62" s="14"/>
-      <c r="G62" s="17"/>
-      <c r="H62" s="56"/>
-      <c r="I62" s="17"/>
-      <c r="J62" s="14"/>
-      <c r="K62" s="58"/>
-      <c r="L62" s="56"/>
-      <c r="M62" s="17"/>
-      <c r="N62" s="14"/>
-      <c r="O62" s="17"/>
-      <c r="P62" s="14"/>
-      <c r="Q62" s="17"/>
-      <c r="R62" s="14"/>
-      <c r="S62" s="23"/>
+      <c r="A62" s="21"/>
+      <c r="B62" s="44"/>
+      <c r="C62" s="46"/>
+      <c r="D62" s="48"/>
+      <c r="E62" s="46"/>
+      <c r="F62" s="48"/>
+      <c r="G62" s="46"/>
+      <c r="H62" s="65"/>
+      <c r="I62" s="46"/>
+      <c r="J62" s="48"/>
+      <c r="K62" s="67"/>
+      <c r="L62" s="65"/>
+      <c r="M62" s="46"/>
+      <c r="N62" s="48"/>
+      <c r="O62" s="46"/>
+      <c r="P62" s="48"/>
+      <c r="Q62" s="46"/>
+      <c r="R62" s="48"/>
+      <c r="S62" s="52"/>
     </row>
     <row r="63" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A63" s="47"/>
-      <c r="B63" s="31" t="s">
+      <c r="A63" s="21"/>
+      <c r="B63" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="C63" s="32" t="s">
+      <c r="C63" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="D63" s="31"/>
-      <c r="E63" s="32"/>
-      <c r="F63" s="31"/>
-      <c r="G63" s="32"/>
-      <c r="H63" s="31"/>
-      <c r="I63" s="32"/>
-      <c r="J63" s="31"/>
-      <c r="K63" s="32"/>
-      <c r="L63" s="31"/>
-      <c r="M63" s="32"/>
-      <c r="N63" s="31"/>
-      <c r="O63" s="32"/>
-      <c r="P63" s="31"/>
-      <c r="Q63" s="32" t="s">
+      <c r="D63" s="7"/>
+      <c r="E63" s="8"/>
+      <c r="F63" s="7"/>
+      <c r="G63" s="8"/>
+      <c r="H63" s="7"/>
+      <c r="I63" s="8"/>
+      <c r="J63" s="7"/>
+      <c r="K63" s="8"/>
+      <c r="L63" s="7"/>
+      <c r="M63" s="8"/>
+      <c r="N63" s="7"/>
+      <c r="O63" s="8"/>
+      <c r="P63" s="7"/>
+      <c r="Q63" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="R63" s="31" t="s">
+      <c r="R63" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="S63" s="37" t="s">
+      <c r="S63" s="13" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="64" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A64" s="47"/>
-      <c r="B64" s="34" t="s">
+      <c r="A64" s="21"/>
+      <c r="B64" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="C64" s="35" t="s">
+      <c r="C64" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="D64" s="38"/>
-      <c r="E64" s="35"/>
-      <c r="F64" s="38"/>
-      <c r="G64" s="35"/>
-      <c r="H64" s="38"/>
-      <c r="I64" s="35"/>
-      <c r="J64" s="38"/>
-      <c r="K64" s="35"/>
-      <c r="L64" s="38"/>
-      <c r="M64" s="35"/>
-      <c r="N64" s="38"/>
-      <c r="O64" s="35"/>
-      <c r="P64" s="38"/>
-      <c r="Q64" s="35"/>
-      <c r="R64" s="38"/>
-      <c r="S64" s="39"/>
+      <c r="D64" s="14"/>
+      <c r="E64" s="11"/>
+      <c r="F64" s="14"/>
+      <c r="G64" s="11"/>
+      <c r="H64" s="14"/>
+      <c r="I64" s="11"/>
+      <c r="J64" s="14"/>
+      <c r="K64" s="11"/>
+      <c r="L64" s="14"/>
+      <c r="M64" s="11"/>
+      <c r="N64" s="14"/>
+      <c r="O64" s="11"/>
+      <c r="P64" s="14"/>
+      <c r="Q64" s="11"/>
+      <c r="R64" s="14"/>
+      <c r="S64" s="15"/>
     </row>
     <row r="65" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A65" s="66"/>
-      <c r="B65" s="74"/>
-      <c r="C65" s="70"/>
-      <c r="D65" s="70"/>
-      <c r="E65" s="70"/>
-      <c r="F65" s="70"/>
-      <c r="G65" s="70"/>
+      <c r="A65" s="34"/>
+      <c r="B65" s="39"/>
+      <c r="C65" s="37"/>
+      <c r="D65" s="37"/>
+      <c r="E65" s="37"/>
+      <c r="F65" s="37"/>
+      <c r="G65" s="37"/>
     </row>
     <row r="66" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A66" s="47"/>
-      <c r="B66" s="9" t="s">
+      <c r="A66" s="21"/>
+      <c r="B66" s="53" t="s">
         <v>114</v>
       </c>
-      <c r="C66" s="69"/>
-      <c r="D66" s="43" t="s">
+      <c r="C66" s="54"/>
+      <c r="D66" s="57" t="s">
         <v>192</v>
       </c>
-      <c r="E66" s="43"/>
-      <c r="F66" s="43"/>
-      <c r="G66" s="44"/>
+      <c r="E66" s="57"/>
+      <c r="F66" s="57"/>
+      <c r="G66" s="58"/>
     </row>
     <row r="67" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A67" s="47"/>
-      <c r="B67" s="12"/>
-      <c r="C67" s="13"/>
-      <c r="D67" s="28" t="s">
+      <c r="A67" s="21"/>
+      <c r="B67" s="55"/>
+      <c r="C67" s="56"/>
+      <c r="D67" s="59" t="s">
         <v>117</v>
       </c>
-      <c r="E67" s="28"/>
-      <c r="F67" s="28"/>
-      <c r="G67" s="29"/>
+      <c r="E67" s="59"/>
+      <c r="F67" s="59"/>
+      <c r="G67" s="60"/>
     </row>
     <row r="68" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="47"/>
-      <c r="B68" s="15" t="s">
+      <c r="A68" s="21"/>
+      <c r="B68" s="43" t="s">
         <v>84</v>
       </c>
-      <c r="C68" s="22" t="s">
+      <c r="C68" s="51" t="s">
         <v>115</v>
       </c>
-      <c r="D68" s="63"/>
-      <c r="E68" s="64"/>
-      <c r="F68" s="64"/>
-      <c r="G68" s="64"/>
+      <c r="D68" s="31"/>
+      <c r="E68" s="32"/>
+      <c r="F68" s="32"/>
+      <c r="G68" s="32"/>
     </row>
     <row r="69" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="47"/>
-      <c r="B69" s="16"/>
-      <c r="C69" s="23"/>
-      <c r="D69" s="62"/>
-      <c r="E69" s="65"/>
-      <c r="F69" s="65"/>
-      <c r="G69" s="65"/>
+      <c r="A69" s="21"/>
+      <c r="B69" s="44"/>
+      <c r="C69" s="52"/>
+      <c r="D69" s="30"/>
+      <c r="E69" s="33"/>
+      <c r="F69" s="33"/>
+      <c r="G69" s="33"/>
     </row>
     <row r="70" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A70" s="47"/>
-      <c r="B70" s="31"/>
-      <c r="C70" s="37"/>
-      <c r="D70" s="42"/>
-      <c r="E70" s="41"/>
-      <c r="F70" s="42"/>
-      <c r="G70" s="41"/>
+      <c r="A70" s="21"/>
+      <c r="B70" s="7"/>
+      <c r="C70" s="13"/>
+      <c r="D70" s="18"/>
+      <c r="E70" s="17"/>
+      <c r="F70" s="18"/>
+      <c r="G70" s="17"/>
     </row>
     <row r="71" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A71" s="47"/>
-      <c r="B71" s="34" t="s">
+      <c r="A71" s="21"/>
+      <c r="B71" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="C71" s="39" t="s">
+      <c r="C71" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="D71" s="46"/>
-      <c r="E71" s="45"/>
-      <c r="F71" s="46"/>
-      <c r="G71" s="45"/>
+      <c r="D71" s="20"/>
+      <c r="E71" s="19"/>
+      <c r="F71" s="20"/>
+      <c r="G71" s="19"/>
       <c r="H71" s="3"/>
     </row>
     <row r="72" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A72" s="66"/>
-      <c r="B72" s="74"/>
+      <c r="A72" s="34"/>
+      <c r="B72" s="39"/>
       <c r="C72" s="2"/>
       <c r="D72" s="2"/>
       <c r="E72" s="2"/>
@@ -3462,235 +3468,239 @@
       <c r="G72" s="2"/>
     </row>
     <row r="73" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A73" s="47"/>
-      <c r="B73" s="9" t="s">
+      <c r="A73" s="21"/>
+      <c r="B73" s="53" t="s">
         <v>127</v>
       </c>
-      <c r="C73" s="69"/>
-      <c r="D73" s="43" t="s">
+      <c r="C73" s="54"/>
+      <c r="D73" s="57" t="s">
         <v>191</v>
       </c>
-      <c r="E73" s="43"/>
-      <c r="F73" s="43"/>
-      <c r="G73" s="44"/>
+      <c r="E73" s="57"/>
+      <c r="F73" s="57"/>
+      <c r="G73" s="58"/>
     </row>
     <row r="74" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A74" s="47"/>
-      <c r="B74" s="12"/>
-      <c r="C74" s="13"/>
-      <c r="D74" s="28" t="s">
+      <c r="A74" s="21"/>
+      <c r="B74" s="55"/>
+      <c r="C74" s="56"/>
+      <c r="D74" s="59" t="s">
         <v>144</v>
       </c>
-      <c r="E74" s="28"/>
-      <c r="F74" s="28"/>
-      <c r="G74" s="29"/>
+      <c r="E74" s="59"/>
+      <c r="F74" s="59"/>
+      <c r="G74" s="60"/>
     </row>
     <row r="75" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="47"/>
-      <c r="B75" s="15" t="s">
+      <c r="A75" s="21"/>
+      <c r="B75" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="C75" s="18" t="s">
+      <c r="C75" s="45" t="s">
         <v>84</v>
       </c>
-      <c r="D75" s="19" t="s">
+      <c r="D75" s="47" t="s">
         <v>118</v>
       </c>
-      <c r="E75" s="18" t="s">
+      <c r="E75" s="45" t="s">
         <v>77</v>
       </c>
-      <c r="F75" s="19" t="s">
+      <c r="F75" s="47" t="s">
         <v>128</v>
       </c>
-      <c r="G75" s="18" t="s">
+      <c r="G75" s="45" t="s">
         <v>129</v>
       </c>
-      <c r="H75" s="19" t="s">
+      <c r="H75" s="47" t="s">
         <v>130</v>
       </c>
-      <c r="I75" s="18" t="s">
+      <c r="I75" s="45" t="s">
         <v>131</v>
       </c>
-      <c r="J75" s="19" t="s">
+      <c r="J75" s="47" t="s">
         <v>135</v>
       </c>
-      <c r="K75" s="18" t="s">
+      <c r="K75" s="45" t="s">
         <v>132</v>
       </c>
-      <c r="L75" s="19" t="s">
+      <c r="L75" s="47" t="s">
         <v>133</v>
       </c>
-      <c r="M75" s="18" t="s">
+      <c r="M75" s="45" t="s">
         <v>134</v>
       </c>
-      <c r="N75" s="19" t="s">
+      <c r="N75" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="O75" s="22" t="s">
+      <c r="O75" s="51" t="s">
         <v>153</v>
       </c>
-      <c r="P75" s="24"/>
-      <c r="Q75" s="24"/>
+      <c r="P75" s="63"/>
+      <c r="Q75" s="63"/>
       <c r="R75" s="3"/>
     </row>
     <row r="76" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="47"/>
-      <c r="B76" s="16"/>
-      <c r="C76" s="17"/>
-      <c r="D76" s="14"/>
-      <c r="E76" s="17"/>
-      <c r="F76" s="14"/>
-      <c r="G76" s="17"/>
-      <c r="H76" s="14"/>
-      <c r="I76" s="26"/>
-      <c r="J76" s="25"/>
-      <c r="K76" s="17"/>
-      <c r="L76" s="14"/>
-      <c r="M76" s="17"/>
-      <c r="N76" s="25"/>
-      <c r="O76" s="23"/>
-      <c r="P76" s="24"/>
-      <c r="Q76" s="24"/>
+      <c r="A76" s="21"/>
+      <c r="B76" s="44"/>
+      <c r="C76" s="46"/>
+      <c r="D76" s="48"/>
+      <c r="E76" s="46"/>
+      <c r="F76" s="48"/>
+      <c r="G76" s="46"/>
+      <c r="H76" s="48"/>
+      <c r="I76" s="49"/>
+      <c r="J76" s="50"/>
+      <c r="K76" s="46"/>
+      <c r="L76" s="48"/>
+      <c r="M76" s="46"/>
+      <c r="N76" s="50"/>
+      <c r="O76" s="52"/>
+      <c r="P76" s="63"/>
+      <c r="Q76" s="63"/>
       <c r="R76" s="3"/>
     </row>
     <row r="77" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A77" s="47"/>
-      <c r="B77" s="31" t="s">
+      <c r="A77" s="21"/>
+      <c r="B77" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C77" s="32"/>
-      <c r="D77" s="31"/>
-      <c r="E77" s="32"/>
-      <c r="F77" s="31"/>
-      <c r="G77" s="32"/>
-      <c r="H77" s="31"/>
-      <c r="I77" s="40"/>
-      <c r="J77" s="31"/>
-      <c r="K77" s="32"/>
-      <c r="L77" s="31"/>
-      <c r="M77" s="32"/>
-      <c r="N77" s="51" t="s">
+      <c r="C77" s="8"/>
+      <c r="D77" s="7"/>
+      <c r="E77" s="8"/>
+      <c r="F77" s="7"/>
+      <c r="G77" s="8"/>
+      <c r="H77" s="7"/>
+      <c r="I77" s="16"/>
+      <c r="J77" s="7"/>
+      <c r="K77" s="8"/>
+      <c r="L77" s="7"/>
+      <c r="M77" s="8"/>
+      <c r="N77" s="25" t="s">
         <v>136</v>
       </c>
-      <c r="O77" s="37"/>
-      <c r="P77" s="46"/>
-      <c r="Q77" s="45"/>
+      <c r="O77" s="13" t="s">
+        <v>258</v>
+      </c>
+      <c r="P77" s="20"/>
+      <c r="Q77" s="19"/>
       <c r="R77" s="3"/>
     </row>
     <row r="78" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A78" s="47"/>
-      <c r="B78" s="34"/>
-      <c r="C78" s="60" t="s">
+      <c r="A78" s="21"/>
+      <c r="B78" s="10"/>
+      <c r="C78" s="28" t="s">
         <v>104</v>
       </c>
-      <c r="D78" s="38" t="s">
+      <c r="D78" s="14" t="s">
         <v>140</v>
       </c>
-      <c r="E78" s="35" t="s">
+      <c r="E78" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="F78" s="38"/>
-      <c r="G78" s="35"/>
-      <c r="H78" s="38"/>
-      <c r="I78" s="35" t="s">
+      <c r="F78" s="14"/>
+      <c r="G78" s="11"/>
+      <c r="H78" s="14"/>
+      <c r="I78" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="J78" s="38" t="s">
+      <c r="J78" s="14" t="s">
         <v>140</v>
       </c>
-      <c r="K78" s="35"/>
-      <c r="L78" s="38"/>
-      <c r="M78" s="35"/>
-      <c r="N78" s="38" t="s">
+      <c r="K78" s="11"/>
+      <c r="L78" s="14"/>
+      <c r="M78" s="11"/>
+      <c r="N78" s="14" t="s">
         <v>138</v>
       </c>
-      <c r="O78" s="39"/>
-      <c r="P78" s="46"/>
-      <c r="Q78" s="45"/>
+      <c r="O78" s="15" t="s">
+        <v>259</v>
+      </c>
+      <c r="P78" s="20"/>
+      <c r="Q78" s="19"/>
       <c r="R78" s="3"/>
     </row>
     <row r="79" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A79" s="66"/>
-      <c r="B79" s="74"/>
-      <c r="C79" s="70"/>
-      <c r="D79" s="70"/>
-      <c r="E79" s="70"/>
-      <c r="F79" s="70"/>
-      <c r="G79" s="70"/>
+      <c r="A79" s="34"/>
+      <c r="B79" s="39"/>
+      <c r="C79" s="37"/>
+      <c r="D79" s="37"/>
+      <c r="E79" s="37"/>
+      <c r="F79" s="37"/>
+      <c r="G79" s="37"/>
     </row>
     <row r="80" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A80" s="47"/>
-      <c r="B80" s="9" t="s">
+      <c r="A80" s="21"/>
+      <c r="B80" s="53" t="s">
         <v>139</v>
       </c>
-      <c r="C80" s="69"/>
-      <c r="D80" s="43" t="s">
+      <c r="C80" s="54"/>
+      <c r="D80" s="57" t="s">
         <v>190</v>
       </c>
-      <c r="E80" s="43"/>
-      <c r="F80" s="43"/>
-      <c r="G80" s="44"/>
+      <c r="E80" s="57"/>
+      <c r="F80" s="57"/>
+      <c r="G80" s="58"/>
     </row>
     <row r="81" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A81" s="47"/>
-      <c r="B81" s="12"/>
-      <c r="C81" s="13"/>
-      <c r="D81" s="28" t="s">
+      <c r="A81" s="21"/>
+      <c r="B81" s="55"/>
+      <c r="C81" s="56"/>
+      <c r="D81" s="59" t="s">
         <v>145</v>
       </c>
-      <c r="E81" s="28"/>
-      <c r="F81" s="28"/>
-      <c r="G81" s="29"/>
+      <c r="E81" s="59"/>
+      <c r="F81" s="59"/>
+      <c r="G81" s="60"/>
     </row>
     <row r="82" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="47"/>
-      <c r="B82" s="15" t="s">
+      <c r="A82" s="21"/>
+      <c r="B82" s="43" t="s">
         <v>115</v>
       </c>
-      <c r="C82" s="18" t="s">
+      <c r="C82" s="45" t="s">
         <v>77</v>
       </c>
-      <c r="D82" s="20" t="s">
+      <c r="D82" s="61" t="s">
         <v>131</v>
       </c>
-      <c r="E82" s="63"/>
-      <c r="F82" s="64"/>
-      <c r="G82" s="64"/>
+      <c r="E82" s="31"/>
+      <c r="F82" s="32"/>
+      <c r="G82" s="32"/>
     </row>
     <row r="83" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="47"/>
-      <c r="B83" s="16"/>
-      <c r="C83" s="17"/>
-      <c r="D83" s="21"/>
-      <c r="E83" s="62"/>
-      <c r="F83" s="65"/>
-      <c r="G83" s="65"/>
+      <c r="A83" s="21"/>
+      <c r="B83" s="44"/>
+      <c r="C83" s="46"/>
+      <c r="D83" s="62"/>
+      <c r="E83" s="30"/>
+      <c r="F83" s="33"/>
+      <c r="G83" s="33"/>
     </row>
     <row r="84" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A84" s="47"/>
-      <c r="B84" s="31"/>
-      <c r="C84" s="32"/>
-      <c r="D84" s="33"/>
-      <c r="E84" s="41"/>
-      <c r="F84" s="42"/>
-      <c r="G84" s="41"/>
+      <c r="A84" s="21"/>
+      <c r="B84" s="7"/>
+      <c r="C84" s="8"/>
+      <c r="D84" s="9"/>
+      <c r="E84" s="17"/>
+      <c r="F84" s="18"/>
+      <c r="G84" s="17"/>
     </row>
     <row r="85" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A85" s="47"/>
-      <c r="B85" s="34" t="s">
+      <c r="A85" s="21"/>
+      <c r="B85" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="C85" s="60" t="s">
+      <c r="C85" s="28" t="s">
         <v>142</v>
       </c>
-      <c r="D85" s="36"/>
-      <c r="E85" s="45"/>
-      <c r="F85" s="46"/>
-      <c r="G85" s="45"/>
+      <c r="D85" s="12"/>
+      <c r="E85" s="19"/>
+      <c r="F85" s="20"/>
+      <c r="G85" s="19"/>
     </row>
     <row r="86" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A86" s="66"/>
-      <c r="B86" s="74"/>
+      <c r="A86" s="34"/>
+      <c r="B86" s="39"/>
       <c r="C86" s="2"/>
       <c r="D86" s="2"/>
       <c r="E86" s="2"/>
@@ -3698,354 +3708,358 @@
       <c r="G86" s="2"/>
     </row>
     <row r="87" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A87" s="47"/>
-      <c r="B87" s="9" t="s">
+      <c r="A87" s="21"/>
+      <c r="B87" s="53" t="s">
         <v>146</v>
       </c>
-      <c r="C87" s="69"/>
-      <c r="D87" s="43" t="s">
+      <c r="C87" s="54"/>
+      <c r="D87" s="57" t="s">
         <v>189</v>
       </c>
-      <c r="E87" s="43"/>
-      <c r="F87" s="43"/>
-      <c r="G87" s="44"/>
+      <c r="E87" s="57"/>
+      <c r="F87" s="57"/>
+      <c r="G87" s="58"/>
     </row>
     <row r="88" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A88" s="47"/>
-      <c r="B88" s="12"/>
-      <c r="C88" s="13"/>
-      <c r="D88" s="28" t="s">
+      <c r="A88" s="21"/>
+      <c r="B88" s="55"/>
+      <c r="C88" s="56"/>
+      <c r="D88" s="59" t="s">
         <v>165</v>
       </c>
-      <c r="E88" s="28"/>
-      <c r="F88" s="28"/>
-      <c r="G88" s="29"/>
+      <c r="E88" s="59"/>
+      <c r="F88" s="59"/>
+      <c r="G88" s="60"/>
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A89" s="47"/>
-      <c r="B89" s="15" t="s">
+      <c r="A89" s="21"/>
+      <c r="B89" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="C89" s="18" t="s">
+      <c r="C89" s="45" t="s">
         <v>115</v>
       </c>
-      <c r="D89" s="19" t="s">
+      <c r="D89" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="E89" s="18" t="s">
+      <c r="E89" s="45" t="s">
         <v>149</v>
       </c>
-      <c r="F89" s="19" t="s">
+      <c r="F89" s="47" t="s">
         <v>130</v>
       </c>
-      <c r="G89" s="18" t="s">
+      <c r="G89" s="45" t="s">
         <v>131</v>
       </c>
-      <c r="H89" s="19" t="s">
+      <c r="H89" s="47" t="s">
         <v>150</v>
       </c>
-      <c r="I89" s="18" t="s">
+      <c r="I89" s="45" t="s">
         <v>151</v>
       </c>
-      <c r="J89" s="19" t="s">
+      <c r="J89" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="K89" s="18" t="s">
+      <c r="K89" s="45" t="s">
         <v>153</v>
       </c>
-      <c r="L89" s="19" t="s">
+      <c r="L89" s="47" t="s">
         <v>154</v>
       </c>
-      <c r="M89" s="18" t="s">
+      <c r="M89" s="45" t="s">
         <v>158</v>
       </c>
-      <c r="N89" s="20" t="s">
+      <c r="N89" s="61" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="90" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A90" s="47"/>
-      <c r="B90" s="16"/>
-      <c r="C90" s="17"/>
-      <c r="D90" s="14"/>
-      <c r="E90" s="17"/>
-      <c r="F90" s="14"/>
-      <c r="G90" s="17"/>
-      <c r="H90" s="14"/>
-      <c r="I90" s="26"/>
-      <c r="J90" s="25"/>
-      <c r="K90" s="17"/>
-      <c r="L90" s="14"/>
-      <c r="M90" s="17"/>
-      <c r="N90" s="21"/>
+      <c r="A90" s="21"/>
+      <c r="B90" s="44"/>
+      <c r="C90" s="46"/>
+      <c r="D90" s="48"/>
+      <c r="E90" s="46"/>
+      <c r="F90" s="48"/>
+      <c r="G90" s="46"/>
+      <c r="H90" s="48"/>
+      <c r="I90" s="49"/>
+      <c r="J90" s="50"/>
+      <c r="K90" s="46"/>
+      <c r="L90" s="48"/>
+      <c r="M90" s="46"/>
+      <c r="N90" s="62"/>
     </row>
     <row r="91" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A91" s="47"/>
-      <c r="B91" s="31" t="s">
+      <c r="A91" s="21"/>
+      <c r="B91" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C91" s="32"/>
-      <c r="D91" s="31"/>
-      <c r="E91" s="32" t="s">
+      <c r="C91" s="8"/>
+      <c r="D91" s="7"/>
+      <c r="E91" s="8" t="s">
         <v>160</v>
       </c>
-      <c r="F91" s="31"/>
-      <c r="G91" s="32"/>
-      <c r="H91" s="31"/>
-      <c r="I91" s="40"/>
-      <c r="J91" s="33" t="s">
+      <c r="F91" s="7"/>
+      <c r="G91" s="8"/>
+      <c r="H91" s="7"/>
+      <c r="I91" s="16"/>
+      <c r="J91" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="K91" s="32"/>
-      <c r="L91" s="31"/>
-      <c r="M91" s="32" t="s">
+      <c r="K91" s="8" t="s">
+        <v>258</v>
+      </c>
+      <c r="L91" s="7"/>
+      <c r="M91" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="N91" s="33"/>
+      <c r="N91" s="9"/>
     </row>
     <row r="92" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A92" s="47"/>
-      <c r="B92" s="34"/>
-      <c r="C92" s="60" t="s">
+      <c r="A92" s="21"/>
+      <c r="B92" s="10"/>
+      <c r="C92" s="28" t="s">
         <v>147</v>
       </c>
-      <c r="D92" s="38" t="s">
+      <c r="D92" s="14" t="s">
         <v>148</v>
       </c>
-      <c r="E92" s="35"/>
-      <c r="F92" s="38"/>
-      <c r="G92" s="35" t="s">
+      <c r="E92" s="11"/>
+      <c r="F92" s="14"/>
+      <c r="G92" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="H92" s="38" t="s">
+      <c r="H92" s="14" t="s">
         <v>161</v>
       </c>
-      <c r="I92" s="60" t="s">
+      <c r="I92" s="28" t="s">
         <v>148</v>
       </c>
-      <c r="J92" s="38" t="s">
+      <c r="J92" s="14" t="s">
         <v>152</v>
       </c>
-      <c r="K92" s="35"/>
-      <c r="L92" s="38" t="s">
+      <c r="K92" s="11" t="s">
+        <v>259</v>
+      </c>
+      <c r="L92" s="14" t="s">
         <v>156</v>
       </c>
-      <c r="M92" s="35"/>
-      <c r="N92" s="36"/>
+      <c r="M92" s="11"/>
+      <c r="N92" s="12"/>
     </row>
     <row r="93" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A93" s="66"/>
-      <c r="B93" s="74"/>
-      <c r="C93" s="70"/>
-      <c r="D93" s="70"/>
-      <c r="E93" s="70"/>
-      <c r="F93" s="70"/>
-      <c r="G93" s="70"/>
+      <c r="A93" s="34"/>
+      <c r="B93" s="39"/>
+      <c r="C93" s="37"/>
+      <c r="D93" s="37"/>
+      <c r="E93" s="37"/>
+      <c r="F93" s="37"/>
+      <c r="G93" s="37"/>
     </row>
     <row r="94" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A94" s="47"/>
-      <c r="B94" s="9" t="s">
+      <c r="A94" s="21"/>
+      <c r="B94" s="53" t="s">
         <v>162</v>
       </c>
-      <c r="C94" s="69"/>
-      <c r="D94" s="43" t="s">
+      <c r="C94" s="54"/>
+      <c r="D94" s="57" t="s">
         <v>188</v>
       </c>
-      <c r="E94" s="43"/>
-      <c r="F94" s="43"/>
-      <c r="G94" s="44"/>
+      <c r="E94" s="57"/>
+      <c r="F94" s="57"/>
+      <c r="G94" s="58"/>
     </row>
     <row r="95" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A95" s="47"/>
-      <c r="B95" s="12"/>
-      <c r="C95" s="13"/>
-      <c r="D95" s="28" t="s">
+      <c r="A95" s="21"/>
+      <c r="B95" s="55"/>
+      <c r="C95" s="56"/>
+      <c r="D95" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="E95" s="28"/>
-      <c r="F95" s="28"/>
-      <c r="G95" s="29"/>
+      <c r="E95" s="59"/>
+      <c r="F95" s="59"/>
+      <c r="G95" s="60"/>
     </row>
     <row r="96" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="47"/>
-      <c r="B96" s="15" t="s">
+      <c r="A96" s="21"/>
+      <c r="B96" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="C96" s="18" t="s">
+      <c r="C96" s="45" t="s">
         <v>170</v>
       </c>
-      <c r="D96" s="19" t="s">
+      <c r="D96" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="E96" s="18" t="s">
+      <c r="E96" s="45" t="s">
         <v>131</v>
       </c>
-      <c r="F96" s="19" t="s">
+      <c r="F96" s="47" t="s">
         <v>163</v>
       </c>
-      <c r="G96" s="18" t="s">
+      <c r="G96" s="45" t="s">
         <v>164</v>
       </c>
-      <c r="H96" s="19" t="s">
+      <c r="H96" s="47" t="s">
         <v>166</v>
       </c>
-      <c r="I96" s="18" t="s">
+      <c r="I96" s="45" t="s">
         <v>167</v>
       </c>
-      <c r="J96" s="20" t="s">
+      <c r="J96" s="61" t="s">
         <v>168</v>
       </c>
-      <c r="K96" s="62"/>
+      <c r="K96" s="30"/>
     </row>
     <row r="97" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="47"/>
-      <c r="B97" s="16"/>
-      <c r="C97" s="17"/>
-      <c r="D97" s="14"/>
-      <c r="E97" s="26"/>
-      <c r="F97" s="25"/>
-      <c r="G97" s="26"/>
-      <c r="H97" s="25"/>
-      <c r="I97" s="26"/>
-      <c r="J97" s="21"/>
-      <c r="K97" s="62"/>
+      <c r="A97" s="21"/>
+      <c r="B97" s="44"/>
+      <c r="C97" s="46"/>
+      <c r="D97" s="48"/>
+      <c r="E97" s="49"/>
+      <c r="F97" s="50"/>
+      <c r="G97" s="49"/>
+      <c r="H97" s="50"/>
+      <c r="I97" s="49"/>
+      <c r="J97" s="62"/>
+      <c r="K97" s="30"/>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A98" s="47"/>
-      <c r="B98" s="31" t="s">
+      <c r="A98" s="21"/>
+      <c r="B98" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C98" s="61" t="s">
+      <c r="C98" s="29" t="s">
         <v>171</v>
       </c>
-      <c r="D98" s="51" t="s">
+      <c r="D98" s="25" t="s">
         <v>169</v>
       </c>
-      <c r="E98" s="32"/>
-      <c r="F98" s="31"/>
-      <c r="G98" s="32"/>
-      <c r="H98" s="31" t="s">
+      <c r="E98" s="8"/>
+      <c r="F98" s="7"/>
+      <c r="G98" s="8"/>
+      <c r="H98" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="I98" s="40" t="s">
+      <c r="I98" s="16" t="s">
         <v>175</v>
       </c>
-      <c r="J98" s="33" t="s">
+      <c r="J98" s="9" t="s">
         <v>176</v>
       </c>
-      <c r="K98" s="45"/>
+      <c r="K98" s="19"/>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A99" s="47"/>
-      <c r="B99" s="34"/>
-      <c r="C99" s="60"/>
-      <c r="D99" s="38"/>
-      <c r="E99" s="35" t="s">
+      <c r="A99" s="21"/>
+      <c r="B99" s="10"/>
+      <c r="C99" s="28"/>
+      <c r="D99" s="14"/>
+      <c r="E99" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="F99" s="38" t="s">
+      <c r="F99" s="14" t="s">
         <v>161</v>
       </c>
-      <c r="G99" s="35" t="s">
+      <c r="G99" s="11" t="s">
         <v>172</v>
       </c>
-      <c r="H99" s="38" t="s">
+      <c r="H99" s="14" t="s">
         <v>173</v>
       </c>
-      <c r="I99" s="60" t="s">
+      <c r="I99" s="28" t="s">
         <v>173</v>
       </c>
-      <c r="J99" s="36" t="s">
+      <c r="J99" s="12" t="s">
         <v>173</v>
       </c>
-      <c r="K99" s="45"/>
+      <c r="K99" s="19"/>
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A100" s="66"/>
-      <c r="B100" s="74"/>
-      <c r="C100" s="70"/>
-      <c r="D100" s="70"/>
-      <c r="E100" s="70"/>
-      <c r="F100" s="70"/>
-      <c r="G100" s="70"/>
+      <c r="A100" s="34"/>
+      <c r="B100" s="39"/>
+      <c r="C100" s="37"/>
+      <c r="D100" s="37"/>
+      <c r="E100" s="37"/>
+      <c r="F100" s="37"/>
+      <c r="G100" s="37"/>
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A101" s="47"/>
-      <c r="B101" s="9" t="s">
+      <c r="A101" s="21"/>
+      <c r="B101" s="53" t="s">
         <v>179</v>
       </c>
-      <c r="C101" s="69"/>
-      <c r="D101" s="43" t="s">
+      <c r="C101" s="54"/>
+      <c r="D101" s="57" t="s">
         <v>187</v>
       </c>
-      <c r="E101" s="43"/>
-      <c r="F101" s="43"/>
-      <c r="G101" s="44"/>
+      <c r="E101" s="57"/>
+      <c r="F101" s="57"/>
+      <c r="G101" s="58"/>
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A102" s="47"/>
-      <c r="B102" s="12"/>
-      <c r="C102" s="13"/>
-      <c r="D102" s="28" t="s">
+      <c r="A102" s="21"/>
+      <c r="B102" s="55"/>
+      <c r="C102" s="56"/>
+      <c r="D102" s="59" t="s">
         <v>155</v>
       </c>
-      <c r="E102" s="28"/>
-      <c r="F102" s="28"/>
-      <c r="G102" s="29"/>
+      <c r="E102" s="59"/>
+      <c r="F102" s="59"/>
+      <c r="G102" s="60"/>
     </row>
     <row r="103" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A103" s="47"/>
-      <c r="B103" s="15" t="s">
+      <c r="A103" s="21"/>
+      <c r="B103" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="C103" s="18" t="s">
+      <c r="C103" s="45" t="s">
         <v>154</v>
       </c>
-      <c r="D103" s="20" t="s">
+      <c r="D103" s="61" t="s">
         <v>177</v>
       </c>
-      <c r="E103" s="64"/>
-      <c r="F103" s="64"/>
-      <c r="G103" s="64"/>
+      <c r="E103" s="32"/>
+      <c r="F103" s="32"/>
+      <c r="G103" s="32"/>
     </row>
     <row r="104" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A104" s="47"/>
-      <c r="B104" s="16"/>
-      <c r="C104" s="26"/>
-      <c r="D104" s="21"/>
-      <c r="E104" s="65"/>
-      <c r="F104" s="65"/>
-      <c r="G104" s="65"/>
+      <c r="A104" s="21"/>
+      <c r="B104" s="44"/>
+      <c r="C104" s="49"/>
+      <c r="D104" s="62"/>
+      <c r="E104" s="33"/>
+      <c r="F104" s="33"/>
+      <c r="G104" s="33"/>
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A105" s="47"/>
-      <c r="B105" s="31" t="s">
+      <c r="A105" s="21"/>
+      <c r="B105" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C105" s="32"/>
-      <c r="D105" s="33" t="s">
+      <c r="C105" s="8"/>
+      <c r="D105" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="E105" s="41"/>
-      <c r="F105" s="42"/>
-      <c r="G105" s="41"/>
+      <c r="E105" s="17"/>
+      <c r="F105" s="18"/>
+      <c r="G105" s="17"/>
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A106" s="47"/>
-      <c r="B106" s="34"/>
-      <c r="C106" s="60" t="s">
+      <c r="A106" s="21"/>
+      <c r="B106" s="10"/>
+      <c r="C106" s="28" t="s">
         <v>155</v>
       </c>
-      <c r="D106" s="36" t="s">
+      <c r="D106" s="12" t="s">
         <v>178</v>
       </c>
-      <c r="E106" s="45"/>
-      <c r="F106" s="46"/>
-      <c r="G106" s="45"/>
+      <c r="E106" s="19"/>
+      <c r="F106" s="20"/>
+      <c r="G106" s="19"/>
     </row>
     <row r="107" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A107" s="66"/>
-      <c r="B107" s="74"/>
+      <c r="A107" s="34"/>
+      <c r="B107" s="39"/>
       <c r="C107" s="2"/>
       <c r="D107" s="2"/>
       <c r="E107" s="2"/>
@@ -4053,923 +4067,892 @@
       <c r="G107" s="2"/>
     </row>
     <row r="108" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A108" s="47"/>
-      <c r="B108" s="9" t="s">
+      <c r="A108" s="21"/>
+      <c r="B108" s="53" t="s">
         <v>181</v>
       </c>
-      <c r="C108" s="69"/>
-      <c r="D108" s="43" t="s">
+      <c r="C108" s="54"/>
+      <c r="D108" s="57" t="s">
         <v>186</v>
       </c>
-      <c r="E108" s="43"/>
-      <c r="F108" s="43"/>
-      <c r="G108" s="44"/>
+      <c r="E108" s="57"/>
+      <c r="F108" s="57"/>
+      <c r="G108" s="58"/>
     </row>
     <row r="109" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A109" s="47"/>
-      <c r="B109" s="12"/>
-      <c r="C109" s="13"/>
-      <c r="D109" s="28" t="s">
+      <c r="A109" s="21"/>
+      <c r="B109" s="55"/>
+      <c r="C109" s="56"/>
+      <c r="D109" s="59" t="s">
         <v>184</v>
       </c>
-      <c r="E109" s="28"/>
-      <c r="F109" s="28"/>
-      <c r="G109" s="29"/>
+      <c r="E109" s="59"/>
+      <c r="F109" s="59"/>
+      <c r="G109" s="60"/>
     </row>
     <row r="110" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A110" s="47"/>
-      <c r="B110" s="15" t="s">
+      <c r="A110" s="21"/>
+      <c r="B110" s="43" t="s">
         <v>182</v>
       </c>
-      <c r="C110" s="22" t="s">
+      <c r="C110" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="D110" s="63"/>
-      <c r="E110" s="64"/>
-      <c r="F110" s="64"/>
-      <c r="G110" s="64"/>
+      <c r="D110" s="31"/>
+      <c r="E110" s="32"/>
+      <c r="F110" s="32"/>
+      <c r="G110" s="32"/>
     </row>
     <row r="111" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A111" s="47"/>
-      <c r="B111" s="16"/>
-      <c r="C111" s="23"/>
-      <c r="D111" s="62"/>
-      <c r="E111" s="65"/>
-      <c r="F111" s="65"/>
-      <c r="G111" s="65"/>
+      <c r="A111" s="21"/>
+      <c r="B111" s="44"/>
+      <c r="C111" s="52"/>
+      <c r="D111" s="30"/>
+      <c r="E111" s="33"/>
+      <c r="F111" s="33"/>
+      <c r="G111" s="33"/>
     </row>
     <row r="112" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A112" s="47"/>
-      <c r="B112" s="31"/>
-      <c r="C112" s="37"/>
-      <c r="D112" s="42"/>
-      <c r="E112" s="41"/>
-      <c r="F112" s="42"/>
-      <c r="G112" s="41"/>
+      <c r="A112" s="21"/>
+      <c r="B112" s="7"/>
+      <c r="C112" s="13"/>
+      <c r="D112" s="18"/>
+      <c r="E112" s="17"/>
+      <c r="F112" s="18"/>
+      <c r="G112" s="17"/>
     </row>
     <row r="113" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A113" s="47"/>
-      <c r="B113" s="34" t="s">
+      <c r="A113" s="21"/>
+      <c r="B113" s="10" t="s">
         <v>183</v>
       </c>
-      <c r="C113" s="39" t="s">
+      <c r="C113" s="15" t="s">
         <v>185</v>
       </c>
-      <c r="D113" s="75"/>
-      <c r="E113" s="45"/>
-      <c r="F113" s="46"/>
-      <c r="G113" s="45"/>
+      <c r="D113" s="40"/>
+      <c r="E113" s="19"/>
+      <c r="F113" s="20"/>
+      <c r="G113" s="19"/>
     </row>
     <row r="114" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A114" s="66"/>
-      <c r="B114" s="74"/>
-      <c r="C114" s="70"/>
+      <c r="A114" s="34"/>
+      <c r="B114" s="39"/>
+      <c r="C114" s="37"/>
       <c r="D114" s="2"/>
       <c r="E114" s="2"/>
       <c r="F114" s="2"/>
       <c r="G114" s="2"/>
     </row>
     <row r="115" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A115" s="47"/>
-      <c r="B115" s="9" t="s">
+      <c r="A115" s="21"/>
+      <c r="B115" s="53" t="s">
         <v>202</v>
       </c>
-      <c r="C115" s="69"/>
-      <c r="D115" s="43" t="s">
+      <c r="C115" s="54"/>
+      <c r="D115" s="57" t="s">
         <v>203</v>
       </c>
-      <c r="E115" s="43"/>
-      <c r="F115" s="43"/>
-      <c r="G115" s="44"/>
+      <c r="E115" s="57"/>
+      <c r="F115" s="57"/>
+      <c r="G115" s="58"/>
     </row>
     <row r="116" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A116" s="47"/>
-      <c r="B116" s="12"/>
-      <c r="C116" s="13"/>
-      <c r="D116" s="28" t="s">
+      <c r="A116" s="21"/>
+      <c r="B116" s="55"/>
+      <c r="C116" s="56"/>
+      <c r="D116" s="59" t="s">
         <v>217</v>
       </c>
-      <c r="E116" s="28"/>
-      <c r="F116" s="28"/>
-      <c r="G116" s="29"/>
+      <c r="E116" s="59"/>
+      <c r="F116" s="59"/>
+      <c r="G116" s="60"/>
     </row>
     <row r="117" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A117" s="47"/>
-      <c r="B117" s="15" t="s">
+      <c r="A117" s="21"/>
+      <c r="B117" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="C117" s="18" t="s">
+      <c r="C117" s="45" t="s">
         <v>112</v>
       </c>
-      <c r="D117" s="19" t="s">
+      <c r="D117" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="E117" s="18" t="s">
+      <c r="E117" s="45" t="s">
         <v>213</v>
       </c>
-      <c r="F117" s="19" t="s">
+      <c r="F117" s="47" t="s">
         <v>149</v>
       </c>
-      <c r="G117" s="18" t="s">
+      <c r="G117" s="45" t="s">
         <v>130</v>
       </c>
-      <c r="H117" s="19" t="s">
+      <c r="H117" s="47" t="s">
         <v>131</v>
       </c>
-      <c r="I117" s="18" t="s">
+      <c r="I117" s="45" t="s">
         <v>158</v>
       </c>
-      <c r="J117" s="19" t="s">
+      <c r="J117" s="47" t="s">
         <v>206</v>
       </c>
-      <c r="K117" s="22" t="s">
+      <c r="K117" s="51" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="118" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A118" s="47"/>
-      <c r="B118" s="16"/>
-      <c r="C118" s="17"/>
-      <c r="D118" s="14"/>
-      <c r="E118" s="26"/>
-      <c r="F118" s="25"/>
-      <c r="G118" s="26"/>
-      <c r="H118" s="25"/>
-      <c r="I118" s="26"/>
-      <c r="J118" s="25"/>
-      <c r="K118" s="23"/>
+      <c r="A118" s="21"/>
+      <c r="B118" s="44"/>
+      <c r="C118" s="46"/>
+      <c r="D118" s="48"/>
+      <c r="E118" s="49"/>
+      <c r="F118" s="50"/>
+      <c r="G118" s="49"/>
+      <c r="H118" s="50"/>
+      <c r="I118" s="49"/>
+      <c r="J118" s="50"/>
+      <c r="K118" s="52"/>
     </row>
     <row r="119" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A119" s="47"/>
-      <c r="B119" s="31" t="s">
+      <c r="A119" s="21"/>
+      <c r="B119" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C119" s="61" t="s">
+      <c r="C119" s="29" t="s">
         <v>204</v>
       </c>
-      <c r="D119" s="51" t="s">
+      <c r="D119" s="25" t="s">
         <v>212</v>
       </c>
-      <c r="E119" s="32" t="s">
+      <c r="E119" s="8" t="s">
         <v>214</v>
       </c>
-      <c r="F119" s="31" t="s">
+      <c r="F119" s="7" t="s">
         <v>210</v>
       </c>
-      <c r="G119" s="32" t="s">
+      <c r="G119" s="8" t="s">
         <v>211</v>
       </c>
-      <c r="H119" s="31"/>
-      <c r="I119" s="40"/>
-      <c r="J119" s="51" t="s">
+      <c r="H119" s="7"/>
+      <c r="I119" s="16"/>
+      <c r="J119" s="25" t="s">
         <v>208</v>
       </c>
-      <c r="K119" s="37" t="s">
+      <c r="K119" s="13" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="120" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A120" s="47"/>
-      <c r="B120" s="34"/>
-      <c r="C120" s="60" t="s">
+      <c r="A120" s="21"/>
+      <c r="B120" s="10"/>
+      <c r="C120" s="28" t="s">
         <v>205</v>
       </c>
-      <c r="D120" s="38" t="s">
+      <c r="D120" s="14" t="s">
         <v>215</v>
       </c>
-      <c r="E120" s="35" t="s">
+      <c r="E120" s="11" t="s">
         <v>216</v>
       </c>
-      <c r="F120" s="38"/>
-      <c r="G120" s="35"/>
-      <c r="H120" s="38" t="s">
+      <c r="F120" s="14"/>
+      <c r="G120" s="11"/>
+      <c r="H120" s="14" t="s">
         <v>161</v>
       </c>
-      <c r="I120" s="60"/>
-      <c r="J120" s="38" t="s">
+      <c r="I120" s="28"/>
+      <c r="J120" s="14" t="s">
         <v>173</v>
       </c>
-      <c r="K120" s="39" t="s">
+      <c r="K120" s="15" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="121" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A121" s="66"/>
-      <c r="B121" s="74"/>
+      <c r="A121" s="34"/>
+      <c r="B121" s="39"/>
       <c r="C121" s="2"/>
       <c r="D121" s="2"/>
       <c r="E121" s="2"/>
       <c r="F121" s="2"/>
       <c r="G121" s="2"/>
-      <c r="K121" s="67"/>
+      <c r="K121" s="35"/>
     </row>
     <row r="122" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A122" s="47"/>
-      <c r="B122" s="9" t="s">
+      <c r="A122" s="21"/>
+      <c r="B122" s="53" t="s">
         <v>218</v>
       </c>
-      <c r="C122" s="69"/>
-      <c r="D122" s="43" t="s">
+      <c r="C122" s="54"/>
+      <c r="D122" s="57" t="s">
         <v>219</v>
       </c>
-      <c r="E122" s="43"/>
-      <c r="F122" s="43"/>
-      <c r="G122" s="44"/>
+      <c r="E122" s="57"/>
+      <c r="F122" s="57"/>
+      <c r="G122" s="58"/>
       <c r="K122" s="3"/>
     </row>
     <row r="123" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A123" s="47"/>
-      <c r="B123" s="12"/>
-      <c r="C123" s="13"/>
-      <c r="D123" s="28" t="s">
+      <c r="A123" s="21"/>
+      <c r="B123" s="55"/>
+      <c r="C123" s="56"/>
+      <c r="D123" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="E123" s="28"/>
-      <c r="F123" s="28"/>
-      <c r="G123" s="29"/>
+      <c r="E123" s="59"/>
+      <c r="F123" s="59"/>
+      <c r="G123" s="60"/>
     </row>
     <row r="124" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A124" s="47"/>
-      <c r="B124" s="15" t="s">
+      <c r="A124" s="21"/>
+      <c r="B124" s="43" t="s">
         <v>220</v>
       </c>
-      <c r="C124" s="22" t="s">
+      <c r="C124" s="51" t="s">
         <v>131</v>
       </c>
-      <c r="D124" s="63"/>
-      <c r="E124" s="64"/>
-      <c r="F124" s="64"/>
-      <c r="G124" s="64"/>
+      <c r="D124" s="31"/>
+      <c r="E124" s="32"/>
+      <c r="F124" s="32"/>
+      <c r="G124" s="32"/>
     </row>
     <row r="125" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A125" s="47"/>
-      <c r="B125" s="16"/>
-      <c r="C125" s="23"/>
-      <c r="D125" s="62"/>
-      <c r="E125" s="65"/>
-      <c r="F125" s="65"/>
-      <c r="G125" s="65"/>
+      <c r="A125" s="21"/>
+      <c r="B125" s="44"/>
+      <c r="C125" s="52"/>
+      <c r="D125" s="30"/>
+      <c r="E125" s="33"/>
+      <c r="F125" s="33"/>
+      <c r="G125" s="33"/>
     </row>
     <row r="126" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A126" s="47"/>
-      <c r="B126" s="31"/>
-      <c r="C126" s="37"/>
-      <c r="D126" s="42"/>
-      <c r="E126" s="41"/>
-      <c r="F126" s="42"/>
-      <c r="G126" s="41"/>
+      <c r="A126" s="21"/>
+      <c r="B126" s="7"/>
+      <c r="C126" s="13"/>
+      <c r="D126" s="18"/>
+      <c r="E126" s="17"/>
+      <c r="F126" s="18"/>
+      <c r="G126" s="17"/>
     </row>
     <row r="127" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A127" s="47"/>
-      <c r="B127" s="76" t="s">
+      <c r="A127" s="21"/>
+      <c r="B127" s="41" t="s">
         <v>221</v>
       </c>
-      <c r="C127" s="39" t="s">
+      <c r="C127" s="15" t="s">
         <v>161</v>
       </c>
-      <c r="D127" s="75"/>
-      <c r="E127" s="45"/>
-      <c r="F127" s="46"/>
-      <c r="G127" s="45"/>
+      <c r="D127" s="40"/>
+      <c r="E127" s="19"/>
+      <c r="F127" s="20"/>
+      <c r="G127" s="19"/>
     </row>
     <row r="128" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A128" s="66"/>
-      <c r="B128" s="74"/>
-      <c r="C128" s="70"/>
+      <c r="A128" s="34"/>
+      <c r="B128" s="39"/>
+      <c r="C128" s="37"/>
       <c r="D128" s="2"/>
       <c r="E128" s="2"/>
       <c r="F128" s="2"/>
       <c r="G128" s="2"/>
     </row>
     <row r="129" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A129" s="47"/>
-      <c r="B129" s="9" t="s">
+      <c r="A129" s="21"/>
+      <c r="B129" s="53" t="s">
         <v>222</v>
       </c>
-      <c r="C129" s="69"/>
-      <c r="D129" s="43" t="s">
+      <c r="C129" s="54"/>
+      <c r="D129" s="57" t="s">
         <v>223</v>
       </c>
-      <c r="E129" s="43"/>
-      <c r="F129" s="43"/>
-      <c r="G129" s="44"/>
+      <c r="E129" s="57"/>
+      <c r="F129" s="57"/>
+      <c r="G129" s="58"/>
     </row>
     <row r="130" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A130" s="47"/>
-      <c r="B130" s="12"/>
-      <c r="C130" s="13"/>
-      <c r="D130" s="28" t="s">
+      <c r="A130" s="21"/>
+      <c r="B130" s="55"/>
+      <c r="C130" s="56"/>
+      <c r="D130" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="E130" s="28"/>
-      <c r="F130" s="28"/>
-      <c r="G130" s="29"/>
+      <c r="E130" s="59"/>
+      <c r="F130" s="59"/>
+      <c r="G130" s="60"/>
     </row>
     <row r="131" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="47"/>
-      <c r="B131" s="15" t="s">
+      <c r="A131" s="21"/>
+      <c r="B131" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="C131" s="18" t="s">
+      <c r="C131" s="45" t="s">
         <v>224</v>
       </c>
-      <c r="D131" s="19" t="s">
+      <c r="D131" s="47" t="s">
         <v>225</v>
       </c>
-      <c r="E131" s="18" t="s">
+      <c r="E131" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="F131" s="20" t="s">
+      <c r="F131" s="61" t="s">
         <v>11</v>
       </c>
-      <c r="G131" s="63"/>
+      <c r="G131" s="31"/>
     </row>
     <row r="132" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="47"/>
-      <c r="B132" s="16"/>
-      <c r="C132" s="17"/>
-      <c r="D132" s="14"/>
-      <c r="E132" s="26"/>
-      <c r="F132" s="21"/>
-      <c r="G132" s="62"/>
+      <c r="A132" s="21"/>
+      <c r="B132" s="44"/>
+      <c r="C132" s="46"/>
+      <c r="D132" s="48"/>
+      <c r="E132" s="49"/>
+      <c r="F132" s="62"/>
+      <c r="G132" s="30"/>
     </row>
     <row r="133" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A133" s="47"/>
-      <c r="B133" s="31" t="s">
+      <c r="A133" s="21"/>
+      <c r="B133" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C133" s="61" t="s">
+      <c r="C133" s="29" t="s">
         <v>226</v>
       </c>
-      <c r="D133" s="51" t="s">
+      <c r="D133" s="25" t="s">
         <v>227</v>
       </c>
-      <c r="E133" s="32" t="s">
+      <c r="E133" s="8" t="s">
         <v>228</v>
       </c>
-      <c r="F133" s="33" t="s">
+      <c r="F133" s="9" t="s">
         <v>229</v>
       </c>
-      <c r="G133" s="41"/>
+      <c r="G133" s="17"/>
     </row>
     <row r="134" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A134" s="47"/>
-      <c r="B134" s="34"/>
-      <c r="C134" s="60" t="s">
+      <c r="A134" s="21"/>
+      <c r="B134" s="10"/>
+      <c r="C134" s="28" t="s">
         <v>178</v>
       </c>
-      <c r="D134" s="38" t="s">
+      <c r="D134" s="14" t="s">
         <v>178</v>
       </c>
-      <c r="E134" s="35" t="s">
+      <c r="E134" s="11" t="s">
         <v>172</v>
       </c>
-      <c r="F134" s="36" t="s">
+      <c r="F134" s="12" t="s">
         <v>178</v>
       </c>
-      <c r="G134" s="45"/>
+      <c r="G134" s="19"/>
     </row>
     <row r="135" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A135" s="66"/>
-      <c r="B135" s="74"/>
-      <c r="C135" s="70"/>
+      <c r="A135" s="34"/>
+      <c r="B135" s="39"/>
+      <c r="C135" s="37"/>
       <c r="D135" s="2"/>
       <c r="E135" s="2"/>
       <c r="F135" s="2"/>
       <c r="G135" s="2"/>
     </row>
     <row r="136" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A136" s="47"/>
-      <c r="B136" s="9" t="s">
+      <c r="A136" s="21"/>
+      <c r="B136" s="53" t="s">
         <v>230</v>
       </c>
-      <c r="C136" s="69"/>
-      <c r="D136" s="43" t="s">
+      <c r="C136" s="54"/>
+      <c r="D136" s="57" t="s">
         <v>231</v>
       </c>
-      <c r="E136" s="43"/>
-      <c r="F136" s="43"/>
-      <c r="G136" s="44"/>
+      <c r="E136" s="57"/>
+      <c r="F136" s="57"/>
+      <c r="G136" s="58"/>
     </row>
     <row r="137" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A137" s="47"/>
-      <c r="B137" s="12"/>
-      <c r="C137" s="13"/>
-      <c r="D137" s="28" t="s">
+      <c r="A137" s="21"/>
+      <c r="B137" s="55"/>
+      <c r="C137" s="56"/>
+      <c r="D137" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="E137" s="28"/>
-      <c r="F137" s="28"/>
-      <c r="G137" s="29"/>
+      <c r="E137" s="59"/>
+      <c r="F137" s="59"/>
+      <c r="G137" s="60"/>
     </row>
     <row r="138" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A138" s="47"/>
-      <c r="B138" s="15" t="s">
+      <c r="A138" s="21"/>
+      <c r="B138" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="C138" s="18" t="s">
+      <c r="C138" s="45" t="s">
         <v>77</v>
       </c>
-      <c r="D138" s="19" t="s">
+      <c r="D138" s="47" t="s">
         <v>236</v>
       </c>
-      <c r="E138" s="18" t="s">
+      <c r="E138" s="45" t="s">
         <v>157</v>
       </c>
-      <c r="F138" s="19" t="s">
+      <c r="F138" s="47" t="s">
         <v>234</v>
       </c>
-      <c r="G138" s="18" t="s">
+      <c r="G138" s="45" t="s">
         <v>235</v>
       </c>
-      <c r="H138" s="19" t="s">
+      <c r="H138" s="47" t="s">
         <v>237</v>
       </c>
-      <c r="I138" s="18" t="s">
+      <c r="I138" s="45" t="s">
         <v>238</v>
       </c>
-      <c r="J138" s="19"/>
-      <c r="K138" s="22"/>
+      <c r="J138" s="47"/>
+      <c r="K138" s="51"/>
     </row>
     <row r="139" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A139" s="47"/>
-      <c r="B139" s="16"/>
-      <c r="C139" s="17"/>
-      <c r="D139" s="14"/>
-      <c r="E139" s="26"/>
-      <c r="F139" s="25"/>
-      <c r="G139" s="26"/>
-      <c r="H139" s="25"/>
-      <c r="I139" s="26"/>
-      <c r="J139" s="25"/>
-      <c r="K139" s="23"/>
+      <c r="A139" s="21"/>
+      <c r="B139" s="44"/>
+      <c r="C139" s="46"/>
+      <c r="D139" s="48"/>
+      <c r="E139" s="49"/>
+      <c r="F139" s="50"/>
+      <c r="G139" s="49"/>
+      <c r="H139" s="50"/>
+      <c r="I139" s="49"/>
+      <c r="J139" s="50"/>
+      <c r="K139" s="52"/>
     </row>
     <row r="140" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A140" s="47"/>
-      <c r="B140" s="31" t="s">
+      <c r="A140" s="21"/>
+      <c r="B140" s="7" t="s">
         <v>232</v>
       </c>
-      <c r="C140" s="61"/>
-      <c r="D140" s="51"/>
-      <c r="E140" s="32"/>
-      <c r="F140" s="31"/>
-      <c r="G140" s="32"/>
-      <c r="H140" s="31" t="s">
+      <c r="C140" s="29"/>
+      <c r="D140" s="25"/>
+      <c r="E140" s="8"/>
+      <c r="F140" s="7"/>
+      <c r="G140" s="8"/>
+      <c r="H140" s="7" t="s">
         <v>242</v>
       </c>
-      <c r="I140" s="40" t="s">
+      <c r="I140" s="16" t="s">
         <v>243</v>
       </c>
-      <c r="J140" s="51"/>
-      <c r="K140" s="37"/>
+      <c r="J140" s="25"/>
+      <c r="K140" s="13"/>
     </row>
     <row r="141" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A141" s="47"/>
-      <c r="B141" s="34" t="s">
+      <c r="A141" s="21"/>
+      <c r="B141" s="10" t="s">
         <v>233</v>
       </c>
-      <c r="C141" s="60" t="s">
+      <c r="C141" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="D141" s="38"/>
-      <c r="E141" s="35"/>
-      <c r="F141" s="38"/>
-      <c r="G141" s="35" t="s">
+      <c r="D141" s="14"/>
+      <c r="E141" s="11"/>
+      <c r="F141" s="14"/>
+      <c r="G141" s="11" t="s">
         <v>241</v>
       </c>
-      <c r="H141" s="38"/>
-      <c r="I141" s="60"/>
-      <c r="J141" s="38"/>
-      <c r="K141" s="39"/>
+      <c r="H141" s="14"/>
+      <c r="I141" s="28"/>
+      <c r="J141" s="14"/>
+      <c r="K141" s="15"/>
     </row>
     <row r="142" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A142" s="66"/>
-      <c r="B142" s="74"/>
-      <c r="C142" s="70"/>
+      <c r="A142" s="34"/>
+      <c r="B142" s="39"/>
+      <c r="C142" s="37"/>
       <c r="D142" s="2"/>
       <c r="E142" s="2"/>
       <c r="F142" s="2"/>
       <c r="G142" s="2"/>
     </row>
     <row r="143" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A143" s="47"/>
-      <c r="B143" s="9" t="s">
+      <c r="A143" s="21"/>
+      <c r="B143" s="53" t="s">
         <v>239</v>
       </c>
-      <c r="C143" s="69"/>
-      <c r="D143" s="43" t="s">
+      <c r="C143" s="54"/>
+      <c r="D143" s="57" t="s">
         <v>240</v>
       </c>
-      <c r="E143" s="43"/>
-      <c r="F143" s="43"/>
-      <c r="G143" s="44"/>
+      <c r="E143" s="57"/>
+      <c r="F143" s="57"/>
+      <c r="G143" s="58"/>
     </row>
     <row r="144" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A144" s="47"/>
-      <c r="B144" s="12"/>
-      <c r="C144" s="13"/>
-      <c r="D144" s="28" t="s">
+      <c r="A144" s="21"/>
+      <c r="B144" s="55"/>
+      <c r="C144" s="56"/>
+      <c r="D144" s="59" t="s">
         <v>76</v>
       </c>
-      <c r="E144" s="28"/>
-      <c r="F144" s="28"/>
-      <c r="G144" s="29"/>
+      <c r="E144" s="59"/>
+      <c r="F144" s="59"/>
+      <c r="G144" s="60"/>
     </row>
     <row r="145" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A145" s="47"/>
-      <c r="B145" s="15" t="s">
+      <c r="A145" s="21"/>
+      <c r="B145" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="C145" s="18" t="s">
+      <c r="C145" s="45" t="s">
         <v>77</v>
       </c>
-      <c r="D145" s="19" t="s">
+      <c r="D145" s="47" t="s">
         <v>236</v>
       </c>
-      <c r="E145" s="18" t="s">
+      <c r="E145" s="45" t="s">
         <v>157</v>
       </c>
-      <c r="F145" s="19" t="s">
+      <c r="F145" s="47" t="s">
         <v>234</v>
       </c>
-      <c r="G145" s="18" t="s">
+      <c r="G145" s="45" t="s">
         <v>235</v>
       </c>
-      <c r="H145" s="19" t="s">
+      <c r="H145" s="47" t="s">
         <v>237</v>
       </c>
-      <c r="I145" s="18"/>
-      <c r="J145" s="19"/>
-      <c r="K145" s="22"/>
+      <c r="I145" s="45"/>
+      <c r="J145" s="47"/>
+      <c r="K145" s="51"/>
     </row>
     <row r="146" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A146" s="47"/>
-      <c r="B146" s="16"/>
-      <c r="C146" s="17"/>
-      <c r="D146" s="14"/>
-      <c r="E146" s="26"/>
-      <c r="F146" s="25"/>
-      <c r="G146" s="26"/>
-      <c r="H146" s="25"/>
-      <c r="I146" s="26"/>
-      <c r="J146" s="25"/>
-      <c r="K146" s="23"/>
+      <c r="A146" s="21"/>
+      <c r="B146" s="44"/>
+      <c r="C146" s="46"/>
+      <c r="D146" s="48"/>
+      <c r="E146" s="49"/>
+      <c r="F146" s="50"/>
+      <c r="G146" s="49"/>
+      <c r="H146" s="50"/>
+      <c r="I146" s="49"/>
+      <c r="J146" s="50"/>
+      <c r="K146" s="52"/>
     </row>
     <row r="147" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A147" s="47"/>
-      <c r="B147" s="31" t="s">
+      <c r="A147" s="21"/>
+      <c r="B147" s="7" t="s">
         <v>232</v>
       </c>
-      <c r="C147" s="61"/>
-      <c r="D147" s="51"/>
-      <c r="E147" s="32"/>
-      <c r="F147" s="31"/>
-      <c r="G147" s="32"/>
-      <c r="H147" s="31" t="s">
+      <c r="C147" s="29"/>
+      <c r="D147" s="25"/>
+      <c r="E147" s="8"/>
+      <c r="F147" s="7"/>
+      <c r="G147" s="8"/>
+      <c r="H147" s="7" t="s">
         <v>242</v>
       </c>
-      <c r="I147" s="40"/>
-      <c r="J147" s="51"/>
-      <c r="K147" s="37"/>
+      <c r="I147" s="16"/>
+      <c r="J147" s="25"/>
+      <c r="K147" s="13"/>
     </row>
     <row r="148" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A148" s="47"/>
-      <c r="B148" s="34" t="s">
+      <c r="A148" s="21"/>
+      <c r="B148" s="10" t="s">
         <v>233</v>
       </c>
-      <c r="C148" s="60" t="s">
+      <c r="C148" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="D148" s="38"/>
-      <c r="E148" s="35"/>
-      <c r="F148" s="38"/>
-      <c r="G148" s="35" t="s">
+      <c r="D148" s="14"/>
+      <c r="E148" s="11"/>
+      <c r="F148" s="14"/>
+      <c r="G148" s="11" t="s">
         <v>241</v>
       </c>
-      <c r="H148" s="38"/>
-      <c r="I148" s="60"/>
-      <c r="J148" s="38"/>
-      <c r="K148" s="39"/>
+      <c r="H148" s="14"/>
+      <c r="I148" s="28"/>
+      <c r="J148" s="14"/>
+      <c r="K148" s="15"/>
     </row>
     <row r="149" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A149" s="66"/>
-      <c r="B149" s="74"/>
-      <c r="C149" s="70"/>
+      <c r="A149" s="34"/>
+      <c r="B149" s="39"/>
+      <c r="C149" s="37"/>
       <c r="D149" s="2"/>
       <c r="E149" s="2"/>
       <c r="F149" s="2"/>
       <c r="G149" s="2"/>
     </row>
     <row r="150" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A150" s="47"/>
-      <c r="B150" s="9" t="s">
+      <c r="A150" s="21"/>
+      <c r="B150" s="53" t="s">
         <v>244</v>
       </c>
-      <c r="C150" s="69"/>
-      <c r="D150" s="43" t="s">
+      <c r="C150" s="54"/>
+      <c r="D150" s="57" t="s">
         <v>245</v>
       </c>
-      <c r="E150" s="43"/>
-      <c r="F150" s="43"/>
-      <c r="G150" s="44"/>
+      <c r="E150" s="57"/>
+      <c r="F150" s="57"/>
+      <c r="G150" s="58"/>
     </row>
     <row r="151" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A151" s="47"/>
-      <c r="B151" s="12"/>
-      <c r="C151" s="13"/>
-      <c r="D151" s="28" t="s">
+      <c r="A151" s="21"/>
+      <c r="B151" s="55"/>
+      <c r="C151" s="56"/>
+      <c r="D151" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="E151" s="28"/>
-      <c r="F151" s="28"/>
-      <c r="G151" s="29"/>
+      <c r="E151" s="59"/>
+      <c r="F151" s="59"/>
+      <c r="G151" s="60"/>
     </row>
     <row r="152" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A152" s="47"/>
-      <c r="B152" s="15" t="s">
+      <c r="A152" s="21"/>
+      <c r="B152" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="C152" s="18" t="s">
+      <c r="C152" s="45" t="s">
         <v>246</v>
       </c>
-      <c r="D152" s="19" t="s">
+      <c r="D152" s="47" t="s">
         <v>247</v>
       </c>
-      <c r="E152" s="22" t="s">
+      <c r="E152" s="51" t="s">
         <v>248</v>
       </c>
-      <c r="F152" s="63"/>
-      <c r="G152" s="64"/>
+      <c r="F152" s="31"/>
+      <c r="G152" s="32"/>
     </row>
     <row r="153" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A153" s="47"/>
-      <c r="B153" s="16"/>
-      <c r="C153" s="17"/>
-      <c r="D153" s="14"/>
-      <c r="E153" s="23"/>
-      <c r="F153" s="62"/>
-      <c r="G153" s="77"/>
+      <c r="A153" s="21"/>
+      <c r="B153" s="44"/>
+      <c r="C153" s="46"/>
+      <c r="D153" s="48"/>
+      <c r="E153" s="52"/>
+      <c r="F153" s="30"/>
+      <c r="G153" s="42"/>
     </row>
     <row r="154" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A154" s="47"/>
-      <c r="B154" s="31" t="s">
+      <c r="A154" s="21"/>
+      <c r="B154" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C154" s="61" t="s">
+      <c r="C154" s="29" t="s">
         <v>249</v>
       </c>
-      <c r="D154" s="51" t="s">
+      <c r="D154" s="25" t="s">
         <v>250</v>
       </c>
-      <c r="E154" s="37" t="s">
+      <c r="E154" s="13" t="s">
         <v>251</v>
       </c>
-      <c r="F154" s="75"/>
-      <c r="G154" s="41"/>
+      <c r="F154" s="40"/>
+      <c r="G154" s="17"/>
     </row>
     <row r="155" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A155" s="47"/>
-      <c r="B155" s="34"/>
-      <c r="C155" s="60" t="s">
+      <c r="A155" s="21"/>
+      <c r="B155" s="10"/>
+      <c r="C155" s="28" t="s">
         <v>178</v>
       </c>
-      <c r="D155" s="38" t="s">
+      <c r="D155" s="14" t="s">
         <v>178</v>
       </c>
-      <c r="E155" s="39" t="s">
+      <c r="E155" s="15" t="s">
         <v>173</v>
       </c>
-      <c r="F155" s="75"/>
-      <c r="G155" s="45"/>
+      <c r="F155" s="40"/>
+      <c r="G155" s="19"/>
     </row>
     <row r="156" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A156" s="66"/>
-      <c r="B156" s="74"/>
-      <c r="C156" s="70"/>
+      <c r="A156" s="34"/>
+      <c r="B156" s="39"/>
+      <c r="C156" s="37"/>
       <c r="D156" s="2"/>
       <c r="E156" s="2"/>
       <c r="F156" s="2"/>
       <c r="G156" s="2"/>
     </row>
     <row r="157" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A157" s="47"/>
-      <c r="B157" s="9" t="s">
+      <c r="A157" s="21"/>
+      <c r="B157" s="53" t="s">
         <v>252</v>
       </c>
-      <c r="C157" s="69"/>
-      <c r="D157" s="43" t="s">
+      <c r="C157" s="54"/>
+      <c r="D157" s="57" t="s">
         <v>253</v>
       </c>
-      <c r="E157" s="43"/>
-      <c r="F157" s="43"/>
-      <c r="G157" s="44"/>
+      <c r="E157" s="57"/>
+      <c r="F157" s="57"/>
+      <c r="G157" s="58"/>
     </row>
     <row r="158" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A158" s="47"/>
-      <c r="B158" s="12"/>
-      <c r="C158" s="13"/>
-      <c r="D158" s="28" t="s">
+      <c r="A158" s="21"/>
+      <c r="B158" s="55"/>
+      <c r="C158" s="56"/>
+      <c r="D158" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="E158" s="28"/>
-      <c r="F158" s="28"/>
-      <c r="G158" s="29"/>
-    </row>
-    <row r="159" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A159" s="47"/>
-      <c r="B159" s="15" t="s">
+      <c r="E158" s="59"/>
+      <c r="F158" s="59"/>
+      <c r="G158" s="60"/>
+    </row>
+    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A159" s="21"/>
+      <c r="B159" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="C159" s="18" t="s">
+      <c r="C159" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="D159" s="19" t="s">
+      <c r="D159" s="47" t="s">
         <v>254</v>
       </c>
-      <c r="E159" s="18" t="s">
+      <c r="E159" s="45" t="s">
         <v>255</v>
       </c>
-      <c r="F159" s="19" t="s">
+      <c r="F159" s="47" t="s">
         <v>256</v>
       </c>
-      <c r="G159" s="22" t="s">
+      <c r="G159" s="51" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="160" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A160" s="47"/>
-      <c r="B160" s="16"/>
-      <c r="C160" s="17"/>
-      <c r="D160" s="14"/>
-      <c r="E160" s="26"/>
-      <c r="F160" s="25"/>
-      <c r="G160" s="23"/>
+    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A160" s="21"/>
+      <c r="B160" s="44"/>
+      <c r="C160" s="46"/>
+      <c r="D160" s="48"/>
+      <c r="E160" s="49"/>
+      <c r="F160" s="50"/>
+      <c r="G160" s="52"/>
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A161" s="47"/>
-      <c r="B161" s="31" t="s">
+      <c r="A161" s="21"/>
+      <c r="B161" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C161" s="61" t="s">
+      <c r="C161" s="29" t="s">
         <v>226</v>
       </c>
-      <c r="D161" s="51" t="s">
+      <c r="D161" s="25" t="s">
         <v>257</v>
       </c>
-      <c r="E161" s="32"/>
-      <c r="F161" s="51"/>
-      <c r="G161" s="37"/>
+      <c r="E161" s="8"/>
+      <c r="F161" s="25"/>
+      <c r="G161" s="13"/>
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A162" s="47"/>
-      <c r="B162" s="34"/>
-      <c r="C162" s="60" t="s">
+      <c r="A162" s="21"/>
+      <c r="B162" s="10"/>
+      <c r="C162" s="28" t="s">
         <v>178</v>
       </c>
-      <c r="D162" s="38" t="s">
+      <c r="D162" s="14" t="s">
         <v>178</v>
       </c>
-      <c r="E162" s="35" t="s">
+      <c r="E162" s="11" t="s">
         <v>178</v>
       </c>
-      <c r="F162" s="38" t="s">
+      <c r="F162" s="14" t="s">
         <v>178</v>
       </c>
-      <c r="G162" s="39" t="s">
+      <c r="G162" s="15" t="s">
         <v>172</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="251">
-    <mergeCell ref="B159:B160"/>
-    <mergeCell ref="C159:C160"/>
-    <mergeCell ref="D159:D160"/>
-    <mergeCell ref="E159:E160"/>
-    <mergeCell ref="F159:F160"/>
-    <mergeCell ref="G159:G160"/>
-    <mergeCell ref="B152:B153"/>
-    <mergeCell ref="C152:C153"/>
-    <mergeCell ref="D152:D153"/>
-    <mergeCell ref="E152:E153"/>
-    <mergeCell ref="B157:C158"/>
-    <mergeCell ref="D157:G157"/>
-    <mergeCell ref="D158:G158"/>
-    <mergeCell ref="H145:H146"/>
-    <mergeCell ref="I145:I146"/>
-    <mergeCell ref="J145:J146"/>
-    <mergeCell ref="K145:K146"/>
-    <mergeCell ref="B150:C151"/>
-    <mergeCell ref="D150:G150"/>
-    <mergeCell ref="D151:G151"/>
-    <mergeCell ref="B145:B146"/>
-    <mergeCell ref="C145:C146"/>
-    <mergeCell ref="D145:D146"/>
-    <mergeCell ref="E145:E146"/>
-    <mergeCell ref="F145:F146"/>
-    <mergeCell ref="G145:G146"/>
-    <mergeCell ref="H138:H139"/>
-    <mergeCell ref="I138:I139"/>
-    <mergeCell ref="J138:J139"/>
-    <mergeCell ref="K138:K139"/>
-    <mergeCell ref="B143:C144"/>
-    <mergeCell ref="D143:G143"/>
-    <mergeCell ref="D144:G144"/>
-    <mergeCell ref="B136:C137"/>
-    <mergeCell ref="D136:G136"/>
-    <mergeCell ref="D137:G137"/>
-    <mergeCell ref="B138:B139"/>
-    <mergeCell ref="C138:C139"/>
-    <mergeCell ref="D138:D139"/>
-    <mergeCell ref="E138:E139"/>
-    <mergeCell ref="F138:F139"/>
-    <mergeCell ref="G138:G139"/>
-    <mergeCell ref="B124:B125"/>
-    <mergeCell ref="C124:C125"/>
-    <mergeCell ref="B129:C130"/>
-    <mergeCell ref="D129:G129"/>
-    <mergeCell ref="D130:G130"/>
-    <mergeCell ref="B131:B132"/>
-    <mergeCell ref="C131:C132"/>
-    <mergeCell ref="D131:D132"/>
-    <mergeCell ref="E131:E132"/>
-    <mergeCell ref="F131:F132"/>
-    <mergeCell ref="G117:G118"/>
-    <mergeCell ref="H117:H118"/>
-    <mergeCell ref="I117:I118"/>
-    <mergeCell ref="J117:J118"/>
-    <mergeCell ref="K117:K118"/>
-    <mergeCell ref="B122:C123"/>
-    <mergeCell ref="D122:G122"/>
-    <mergeCell ref="D123:G123"/>
-    <mergeCell ref="B110:B111"/>
-    <mergeCell ref="C110:C111"/>
-    <mergeCell ref="B115:C116"/>
-    <mergeCell ref="D115:G115"/>
-    <mergeCell ref="D116:G116"/>
-    <mergeCell ref="B117:B118"/>
-    <mergeCell ref="C117:C118"/>
-    <mergeCell ref="D117:D118"/>
-    <mergeCell ref="E117:E118"/>
-    <mergeCell ref="F117:F118"/>
-    <mergeCell ref="B103:B104"/>
-    <mergeCell ref="C103:C104"/>
-    <mergeCell ref="D103:D104"/>
-    <mergeCell ref="B108:C109"/>
-    <mergeCell ref="D108:G108"/>
-    <mergeCell ref="D109:G109"/>
-    <mergeCell ref="H96:H97"/>
-    <mergeCell ref="I96:I97"/>
-    <mergeCell ref="J96:J97"/>
-    <mergeCell ref="B101:C102"/>
-    <mergeCell ref="D101:G101"/>
-    <mergeCell ref="D102:G102"/>
-    <mergeCell ref="N89:N90"/>
-    <mergeCell ref="B94:C95"/>
-    <mergeCell ref="D94:G94"/>
-    <mergeCell ref="D95:G95"/>
-    <mergeCell ref="B96:B97"/>
-    <mergeCell ref="C96:C97"/>
-    <mergeCell ref="D96:D97"/>
-    <mergeCell ref="E96:E97"/>
-    <mergeCell ref="F96:F97"/>
-    <mergeCell ref="G96:G97"/>
-    <mergeCell ref="H89:H90"/>
-    <mergeCell ref="I89:I90"/>
-    <mergeCell ref="J89:J90"/>
-    <mergeCell ref="K89:K90"/>
-    <mergeCell ref="L89:L90"/>
-    <mergeCell ref="M89:M90"/>
-    <mergeCell ref="B87:C88"/>
-    <mergeCell ref="D87:G87"/>
-    <mergeCell ref="D88:G88"/>
-    <mergeCell ref="B89:B90"/>
-    <mergeCell ref="C89:C90"/>
-    <mergeCell ref="D89:D90"/>
-    <mergeCell ref="E89:E90"/>
-    <mergeCell ref="F89:F90"/>
-    <mergeCell ref="G89:G90"/>
-    <mergeCell ref="B82:B83"/>
-    <mergeCell ref="C82:C83"/>
-    <mergeCell ref="D82:D83"/>
-    <mergeCell ref="N75:N76"/>
-    <mergeCell ref="O75:O76"/>
-    <mergeCell ref="P75:P76"/>
-    <mergeCell ref="Q75:Q76"/>
-    <mergeCell ref="B80:C81"/>
-    <mergeCell ref="D80:G80"/>
-    <mergeCell ref="D81:G81"/>
-    <mergeCell ref="H75:H76"/>
-    <mergeCell ref="I75:I76"/>
-    <mergeCell ref="J75:J76"/>
-    <mergeCell ref="K75:K76"/>
-    <mergeCell ref="L75:L76"/>
-    <mergeCell ref="M75:M76"/>
-    <mergeCell ref="B75:B76"/>
-    <mergeCell ref="C75:C76"/>
-    <mergeCell ref="D75:D76"/>
-    <mergeCell ref="E75:E76"/>
-    <mergeCell ref="F75:F76"/>
-    <mergeCell ref="G75:G76"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="B45:C46"/>
+    <mergeCell ref="B24:C25"/>
+    <mergeCell ref="B10:C11"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B3:C4"/>
+    <mergeCell ref="D3:G3"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="D18:G18"/>
+    <mergeCell ref="D45:G45"/>
+    <mergeCell ref="D46:G46"/>
+    <mergeCell ref="D10:G10"/>
+    <mergeCell ref="D11:G11"/>
+    <mergeCell ref="B17:C18"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="H33:H34"/>
+    <mergeCell ref="I33:I34"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="G33:G34"/>
+    <mergeCell ref="D24:G24"/>
+    <mergeCell ref="D25:G25"/>
+    <mergeCell ref="B31:C32"/>
+    <mergeCell ref="D31:G31"/>
+    <mergeCell ref="D32:G32"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="F33:F34"/>
+    <mergeCell ref="D17:G17"/>
+    <mergeCell ref="J33:J34"/>
+    <mergeCell ref="K33:K34"/>
+    <mergeCell ref="L33:L34"/>
+    <mergeCell ref="M33:M34"/>
+    <mergeCell ref="B52:C53"/>
+    <mergeCell ref="D52:G52"/>
+    <mergeCell ref="D53:G53"/>
+    <mergeCell ref="J47:J48"/>
+    <mergeCell ref="K47:K48"/>
+    <mergeCell ref="L47:L48"/>
+    <mergeCell ref="B38:C39"/>
+    <mergeCell ref="D38:G38"/>
+    <mergeCell ref="D39:G39"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="D40:D41"/>
+    <mergeCell ref="H47:H48"/>
+    <mergeCell ref="I47:I48"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="C47:C48"/>
+    <mergeCell ref="D47:D48"/>
+    <mergeCell ref="E47:E48"/>
+    <mergeCell ref="F47:F48"/>
+    <mergeCell ref="G47:G48"/>
+    <mergeCell ref="R54:R55"/>
+    <mergeCell ref="S54:S55"/>
+    <mergeCell ref="H54:H55"/>
+    <mergeCell ref="I54:I55"/>
+    <mergeCell ref="J54:J55"/>
+    <mergeCell ref="K54:K55"/>
+    <mergeCell ref="L54:L55"/>
+    <mergeCell ref="M54:M55"/>
+    <mergeCell ref="N54:N55"/>
+    <mergeCell ref="O54:O55"/>
+    <mergeCell ref="K61:K62"/>
+    <mergeCell ref="L61:L62"/>
+    <mergeCell ref="P54:P55"/>
+    <mergeCell ref="Q54:Q55"/>
+    <mergeCell ref="B59:C60"/>
+    <mergeCell ref="D59:G59"/>
+    <mergeCell ref="D60:G60"/>
+    <mergeCell ref="B61:B62"/>
+    <mergeCell ref="C61:C62"/>
+    <mergeCell ref="D61:D62"/>
+    <mergeCell ref="E61:E62"/>
+    <mergeCell ref="F61:F62"/>
+    <mergeCell ref="B54:B55"/>
+    <mergeCell ref="C54:C55"/>
+    <mergeCell ref="D54:D55"/>
+    <mergeCell ref="E54:E55"/>
+    <mergeCell ref="F54:F55"/>
+    <mergeCell ref="G54:G55"/>
     <mergeCell ref="M47:M48"/>
     <mergeCell ref="N47:N48"/>
     <mergeCell ref="O47:O48"/>
@@ -4994,104 +4977,135 @@
     <mergeCell ref="H61:H62"/>
     <mergeCell ref="I61:I62"/>
     <mergeCell ref="J61:J62"/>
-    <mergeCell ref="K61:K62"/>
-    <mergeCell ref="L61:L62"/>
-    <mergeCell ref="P54:P55"/>
-    <mergeCell ref="Q54:Q55"/>
-    <mergeCell ref="B59:C60"/>
-    <mergeCell ref="D59:G59"/>
-    <mergeCell ref="D60:G60"/>
-    <mergeCell ref="B61:B62"/>
-    <mergeCell ref="C61:C62"/>
-    <mergeCell ref="D61:D62"/>
-    <mergeCell ref="E61:E62"/>
-    <mergeCell ref="F61:F62"/>
-    <mergeCell ref="R54:R55"/>
-    <mergeCell ref="S54:S55"/>
-    <mergeCell ref="H54:H55"/>
-    <mergeCell ref="I54:I55"/>
-    <mergeCell ref="J54:J55"/>
-    <mergeCell ref="K54:K55"/>
-    <mergeCell ref="L54:L55"/>
-    <mergeCell ref="M54:M55"/>
-    <mergeCell ref="N54:N55"/>
-    <mergeCell ref="O54:O55"/>
-    <mergeCell ref="B54:B55"/>
-    <mergeCell ref="C54:C55"/>
-    <mergeCell ref="D54:D55"/>
-    <mergeCell ref="E54:E55"/>
-    <mergeCell ref="F54:F55"/>
-    <mergeCell ref="G54:G55"/>
-    <mergeCell ref="J33:J34"/>
-    <mergeCell ref="K33:K34"/>
-    <mergeCell ref="L33:L34"/>
-    <mergeCell ref="M33:M34"/>
-    <mergeCell ref="B52:C53"/>
-    <mergeCell ref="D52:G52"/>
-    <mergeCell ref="D53:G53"/>
-    <mergeCell ref="J47:J48"/>
-    <mergeCell ref="K47:K48"/>
-    <mergeCell ref="L47:L48"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="H33:H34"/>
-    <mergeCell ref="I33:I34"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="G33:G34"/>
-    <mergeCell ref="B38:C39"/>
-    <mergeCell ref="D38:G38"/>
-    <mergeCell ref="D39:G39"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="D40:D41"/>
-    <mergeCell ref="D24:G24"/>
-    <mergeCell ref="D25:G25"/>
-    <mergeCell ref="B31:C32"/>
-    <mergeCell ref="D31:G31"/>
-    <mergeCell ref="D32:G32"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="F33:F34"/>
-    <mergeCell ref="D17:G17"/>
-    <mergeCell ref="D18:G18"/>
-    <mergeCell ref="D45:G45"/>
-    <mergeCell ref="D46:G46"/>
-    <mergeCell ref="D10:G10"/>
-    <mergeCell ref="D11:G11"/>
-    <mergeCell ref="B17:C18"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="H47:H48"/>
-    <mergeCell ref="I47:I48"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="C47:C48"/>
-    <mergeCell ref="D47:D48"/>
-    <mergeCell ref="E47:E48"/>
-    <mergeCell ref="F47:F48"/>
-    <mergeCell ref="G47:G48"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="B45:C46"/>
-    <mergeCell ref="B24:C25"/>
-    <mergeCell ref="B10:C11"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B3:C4"/>
-    <mergeCell ref="D3:G3"/>
-    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="B82:B83"/>
+    <mergeCell ref="C82:C83"/>
+    <mergeCell ref="D82:D83"/>
+    <mergeCell ref="N75:N76"/>
+    <mergeCell ref="O75:O76"/>
+    <mergeCell ref="P75:P76"/>
+    <mergeCell ref="Q75:Q76"/>
+    <mergeCell ref="B80:C81"/>
+    <mergeCell ref="D80:G80"/>
+    <mergeCell ref="D81:G81"/>
+    <mergeCell ref="H75:H76"/>
+    <mergeCell ref="I75:I76"/>
+    <mergeCell ref="J75:J76"/>
+    <mergeCell ref="K75:K76"/>
+    <mergeCell ref="L75:L76"/>
+    <mergeCell ref="M75:M76"/>
+    <mergeCell ref="B75:B76"/>
+    <mergeCell ref="C75:C76"/>
+    <mergeCell ref="D75:D76"/>
+    <mergeCell ref="E75:E76"/>
+    <mergeCell ref="F75:F76"/>
+    <mergeCell ref="G75:G76"/>
+    <mergeCell ref="B87:C88"/>
+    <mergeCell ref="D87:G87"/>
+    <mergeCell ref="D88:G88"/>
+    <mergeCell ref="B89:B90"/>
+    <mergeCell ref="C89:C90"/>
+    <mergeCell ref="D89:D90"/>
+    <mergeCell ref="E89:E90"/>
+    <mergeCell ref="F89:F90"/>
+    <mergeCell ref="G89:G90"/>
+    <mergeCell ref="N89:N90"/>
+    <mergeCell ref="B94:C95"/>
+    <mergeCell ref="D94:G94"/>
+    <mergeCell ref="D95:G95"/>
+    <mergeCell ref="B96:B97"/>
+    <mergeCell ref="C96:C97"/>
+    <mergeCell ref="D96:D97"/>
+    <mergeCell ref="E96:E97"/>
+    <mergeCell ref="F96:F97"/>
+    <mergeCell ref="G96:G97"/>
+    <mergeCell ref="H89:H90"/>
+    <mergeCell ref="I89:I90"/>
+    <mergeCell ref="J89:J90"/>
+    <mergeCell ref="K89:K90"/>
+    <mergeCell ref="L89:L90"/>
+    <mergeCell ref="M89:M90"/>
+    <mergeCell ref="B103:B104"/>
+    <mergeCell ref="C103:C104"/>
+    <mergeCell ref="D103:D104"/>
+    <mergeCell ref="B108:C109"/>
+    <mergeCell ref="D108:G108"/>
+    <mergeCell ref="D109:G109"/>
+    <mergeCell ref="H96:H97"/>
+    <mergeCell ref="I96:I97"/>
+    <mergeCell ref="J96:J97"/>
+    <mergeCell ref="B101:C102"/>
+    <mergeCell ref="D101:G101"/>
+    <mergeCell ref="D102:G102"/>
+    <mergeCell ref="G117:G118"/>
+    <mergeCell ref="H117:H118"/>
+    <mergeCell ref="I117:I118"/>
+    <mergeCell ref="J117:J118"/>
+    <mergeCell ref="K117:K118"/>
+    <mergeCell ref="B122:C123"/>
+    <mergeCell ref="D122:G122"/>
+    <mergeCell ref="D123:G123"/>
+    <mergeCell ref="B110:B111"/>
+    <mergeCell ref="C110:C111"/>
+    <mergeCell ref="B115:C116"/>
+    <mergeCell ref="D115:G115"/>
+    <mergeCell ref="D116:G116"/>
+    <mergeCell ref="B117:B118"/>
+    <mergeCell ref="C117:C118"/>
+    <mergeCell ref="D117:D118"/>
+    <mergeCell ref="E117:E118"/>
+    <mergeCell ref="F117:F118"/>
+    <mergeCell ref="B124:B125"/>
+    <mergeCell ref="C124:C125"/>
+    <mergeCell ref="B129:C130"/>
+    <mergeCell ref="D129:G129"/>
+    <mergeCell ref="D130:G130"/>
+    <mergeCell ref="B131:B132"/>
+    <mergeCell ref="C131:C132"/>
+    <mergeCell ref="D131:D132"/>
+    <mergeCell ref="E131:E132"/>
+    <mergeCell ref="F131:F132"/>
+    <mergeCell ref="H138:H139"/>
+    <mergeCell ref="I138:I139"/>
+    <mergeCell ref="J138:J139"/>
+    <mergeCell ref="K138:K139"/>
+    <mergeCell ref="B143:C144"/>
+    <mergeCell ref="D143:G143"/>
+    <mergeCell ref="D144:G144"/>
+    <mergeCell ref="B136:C137"/>
+    <mergeCell ref="D136:G136"/>
+    <mergeCell ref="D137:G137"/>
+    <mergeCell ref="B138:B139"/>
+    <mergeCell ref="C138:C139"/>
+    <mergeCell ref="D138:D139"/>
+    <mergeCell ref="E138:E139"/>
+    <mergeCell ref="F138:F139"/>
+    <mergeCell ref="G138:G139"/>
+    <mergeCell ref="H145:H146"/>
+    <mergeCell ref="I145:I146"/>
+    <mergeCell ref="J145:J146"/>
+    <mergeCell ref="K145:K146"/>
+    <mergeCell ref="B150:C151"/>
+    <mergeCell ref="D150:G150"/>
+    <mergeCell ref="D151:G151"/>
+    <mergeCell ref="B145:B146"/>
+    <mergeCell ref="C145:C146"/>
+    <mergeCell ref="D145:D146"/>
+    <mergeCell ref="E145:E146"/>
+    <mergeCell ref="F145:F146"/>
+    <mergeCell ref="G145:G146"/>
+    <mergeCell ref="B159:B160"/>
+    <mergeCell ref="C159:C160"/>
+    <mergeCell ref="D159:D160"/>
+    <mergeCell ref="E159:E160"/>
+    <mergeCell ref="F159:F160"/>
+    <mergeCell ref="G159:G160"/>
+    <mergeCell ref="B152:B153"/>
+    <mergeCell ref="C152:C153"/>
+    <mergeCell ref="D152:D153"/>
+    <mergeCell ref="E152:E153"/>
+    <mergeCell ref="B157:C158"/>
+    <mergeCell ref="D157:G157"/>
+    <mergeCell ref="D158:G158"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>